<commit_message>
implemented --noannotation and --lastzonly
</commit_message>
<xml_diff>
--- a/ddprimer/test_data/Primers/Primers_fasta1.xlsx
+++ b/ddprimer/test_data/Primers/Primers_fasta1.xlsx
@@ -80,7 +80,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -100,9 +100,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z20"/>
+  <dimension ref="A1:Z21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -671,7 +668,7 @@
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
         <is>
-          <t>PDH-E1 ALPHA</t>
+          <t>CP002684.1</t>
         </is>
       </c>
       <c r="B3" s="7" t="inlineStr">
@@ -751,21 +748,17 @@
       <c r="X3" s="6" t="n">
         <v>-8.800433158874512</v>
       </c>
-      <c r="Y3" s="6" t="inlineStr">
-        <is>
-          <t>CP002684.1</t>
-        </is>
-      </c>
+      <c r="Y3" s="6" t="inlineStr"/>
       <c r="Z3" s="6" t="inlineStr">
         <is>
-          <t>48586</t>
+          <t>13</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
         <is>
-          <t>PDH-E1 ALPHA</t>
+          <t>CP002684.1</t>
         </is>
       </c>
       <c r="B4" s="7" t="inlineStr">
@@ -845,239 +838,229 @@
       <c r="X4" s="6" t="n">
         <v>-8.800433158874512</v>
       </c>
-      <c r="Y4" s="6" t="inlineStr">
-        <is>
-          <t>CP002684.1</t>
-        </is>
-      </c>
+      <c r="Y4" s="6" t="inlineStr"/>
       <c r="Z4" s="6" t="inlineStr">
         <is>
-          <t>48598</t>
+          <t>25</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
         <is>
-          <t>CYP703A2</t>
+          <t>CP002684.1</t>
         </is>
       </c>
       <c r="B5" s="7" t="inlineStr">
         <is>
-          <t>GAACGATCCCGATACCATC</t>
+          <t>GAATCTAATCCGCCGAGTC</t>
         </is>
       </c>
       <c r="C5" s="6" t="n">
-        <v>57.18013716608459</v>
+        <v>57.49691898952096</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>1.385652307599617</v>
+        <v>1.068870484163245</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>-0.8097348213195801</v>
+        <v>0</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>0.007</v>
       </c>
-      <c r="G5" s="6" t="inlineStr"/>
+      <c r="G5" s="6" t="n">
+        <v>3.7</v>
+      </c>
       <c r="H5" s="7" t="inlineStr">
         <is>
-          <t>CACATCCATACGCTAGGTG</t>
+          <t>CGCATAGAATCTGAGTCTCC</t>
         </is>
       </c>
       <c r="I5" s="6" t="n">
-        <v>57.40147050241876</v>
+        <v>57.39128463697756</v>
       </c>
       <c r="J5" s="6" t="n">
-        <v>1.164318971265448</v>
+        <v>1.358715363022441</v>
       </c>
       <c r="K5" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L5" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="M5" s="6" t="n">
-        <v>3.7</v>
+        <v>1.1</v>
       </c>
       <c r="N5" s="6" t="n">
-        <v>2.549971278865065</v>
+        <v>2.427585847185686</v>
       </c>
       <c r="O5" s="7" t="inlineStr">
         <is>
-          <t>TCGAGACCCAAAACACTCGCCGCAGT</t>
+          <t>CCGACGCGCCGAGAAAACTCCCG</t>
         </is>
       </c>
       <c r="P5" s="6" t="n">
-        <v>64.30135325099201</v>
+        <v>64.42590694670616</v>
       </c>
       <c r="Q5" s="6" t="n">
-        <v>6.698646749007992</v>
+        <v>3.574093053293836</v>
       </c>
       <c r="R5" s="6" t="n">
-        <v>-1.419864654541016</v>
+        <v>0</v>
       </c>
       <c r="S5" s="6" t="n">
-        <v>1.51e-06</v>
+        <v>4.81e-05</v>
       </c>
       <c r="T5" s="6" t="n">
-        <v>1.4</v>
+        <v>1.1</v>
       </c>
       <c r="U5" s="7" t="inlineStr">
         <is>
-          <t>GAACGATCCCGATACCATCCGTGAGATTCTTTTGCGGCAGGACGATGTTTTTTCATCGAGACCCAAAACACTCGCCGCAGTCCACCTAGCGTATGGATGTGG</t>
+          <t>GAATCTAATCCGCCGAGTCAAACCTAAGACGATCGTCGAAGTCGGGAGTTTTCTCGGCGCGTCGGCGATACACATGGCGAATCTCACGCGCCGACTTGGGCTCGAGGAGACTCAGATTCTATGCGT</t>
         </is>
       </c>
       <c r="V5" s="6" t="n">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="W5" s="6" t="n">
-        <v>51.9607843137255</v>
+        <v>55.55555555555556</v>
       </c>
       <c r="X5" s="6" t="n">
-        <v>-5.947404861450195</v>
-      </c>
-      <c r="Y5" s="6" t="inlineStr">
-        <is>
-          <t>CP002684.1</t>
-        </is>
-      </c>
+        <v>-12.9314661026001</v>
+      </c>
+      <c r="Y5" s="6" t="inlineStr"/>
       <c r="Z5" s="6" t="inlineStr">
         <is>
-          <t>112527</t>
+          <t>10</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
         <is>
-          <t>CYP703A2</t>
+          <t>CP002684.1</t>
         </is>
       </c>
       <c r="B6" s="7" t="inlineStr">
         <is>
-          <t>CAACGAACGATCCCGATAC</t>
+          <t>CCGAGTCAAACCTAAGACG</t>
         </is>
       </c>
       <c r="C6" s="6" t="n">
-        <v>58.1158368244387</v>
+        <v>57.57714328942353</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>1.681626298122911</v>
+        <v>1.142932763107741</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>-0.8097348213195801</v>
+        <v>0</v>
       </c>
       <c r="F6" s="6" t="n">
         <v>0.007</v>
       </c>
       <c r="G6" s="6" t="n">
-        <v>3.7</v>
+        <v>1.1</v>
       </c>
       <c r="H6" s="7" t="inlineStr">
         <is>
-          <t>ATCCATACGCTAGGTGGAC</t>
+          <t>AGAATCTGAGTCTCCTCGAG</t>
         </is>
       </c>
       <c r="I6" s="6" t="n">
-        <v>58.25082796726878</v>
+        <v>57.76917945968336</v>
       </c>
       <c r="J6" s="6" t="n">
-        <v>1.816617440952985</v>
+        <v>1.519179459683357</v>
       </c>
       <c r="K6" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L6" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="M6" s="6" t="n">
         <v>1.1</v>
       </c>
       <c r="N6" s="6" t="n">
-        <v>3.498243739075896</v>
+        <v>2.662112222791098</v>
       </c>
       <c r="O6" s="7" t="inlineStr">
         <is>
-          <t>TCATCGAGACCCAAAACACTCGCCGCA</t>
+          <t>CCGACGCGCCGAGAAAACTCCCG</t>
         </is>
       </c>
       <c r="P6" s="6" t="n">
-        <v>64.20487603053124</v>
+        <v>64.42590694670616</v>
       </c>
       <c r="Q6" s="6" t="n">
-        <v>7.795123969468762</v>
+        <v>3.574093053293836</v>
       </c>
       <c r="R6" s="6" t="n">
-        <v>-1.419864654541016</v>
+        <v>0</v>
       </c>
       <c r="S6" s="6" t="n">
-        <v>5.4e-07</v>
+        <v>4.81e-05</v>
       </c>
       <c r="T6" s="6" t="n">
-        <v>0.042</v>
+        <v>1.1</v>
       </c>
       <c r="U6" s="7" t="inlineStr">
         <is>
-          <t>CAACGAACGATCCCGATACCATCCGTGAGATTCTTTTGCGGCAGGACGATGTTTTTTCATCGAGACCCAAAACACTCGCCGCAGTCCACCTAGCGTATGGATG</t>
+          <t>CCGAGTCAAACCTAAGACGATCGTCGAAGTCGGGAGTTTTCTCGGCGCGTCGGCGATACACATGGCGAATCTCACGCGCCGACTTGGGCTCGAGGAGACTCAGATTCTA</t>
         </is>
       </c>
       <c r="V6" s="6" t="n">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="W6" s="6" t="n">
-        <v>51.45631067961165</v>
+        <v>56.88073394495413</v>
       </c>
       <c r="X6" s="6" t="n">
-        <v>-5.947404861450195</v>
-      </c>
-      <c r="Y6" s="6" t="inlineStr">
-        <is>
-          <t>CP002684.1</t>
-        </is>
-      </c>
+        <v>-12.9314661026001</v>
+      </c>
+      <c r="Y6" s="6" t="inlineStr"/>
       <c r="Z6" s="6" t="inlineStr">
         <is>
-          <t>112523</t>
+          <t>22</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
         <is>
-          <t>At17.1</t>
+          <t>CP002684.1</t>
         </is>
       </c>
       <c r="B7" s="7" t="inlineStr">
         <is>
-          <t>GTCTTCCGATCTCTCCATAC</t>
+          <t>CTAATCCGCCGAGTCAAAC</t>
         </is>
       </c>
       <c r="C7" s="6" t="n">
-        <v>56.72627428247569</v>
+        <v>58.31982523388075</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>2.023725717524314</v>
+        <v>1.885614707564958</v>
       </c>
       <c r="E7" s="6" t="n">
         <v>0</v>
       </c>
       <c r="F7" s="6" t="n">
-        <v>0.002</v>
+        <v>0.007</v>
       </c>
       <c r="G7" s="6" t="n">
-        <v>0.3</v>
+        <v>3.7</v>
       </c>
       <c r="H7" s="7" t="inlineStr">
         <is>
-          <t>CTCAGCTTTGGGAATCCTC</t>
+          <t>CGTCGACGCATAGAATCTG</t>
         </is>
       </c>
       <c r="I7" s="6" t="n">
-        <v>57.50429449531657</v>
+        <v>58.20901248311378</v>
       </c>
       <c r="J7" s="6" t="n">
-        <v>1.07008396900078</v>
+        <v>1.77480195679799</v>
       </c>
       <c r="K7" s="6" t="n">
         <v>0</v>
@@ -1089,89 +1072,83 @@
         <v>1.1</v>
       </c>
       <c r="N7" s="6" t="n">
-        <v>3.093809686525095</v>
+        <v>3.660416664362948</v>
       </c>
       <c r="O7" s="7" t="inlineStr">
         <is>
-          <t>CCTCCGTCGTCCATCCTCCTGGTGGT</t>
+          <t>CCGACGCGCCGAGAAAACTCCCG</t>
         </is>
       </c>
       <c r="P7" s="6" t="n">
-        <v>64.72158538224431</v>
+        <v>64.42590694670616</v>
       </c>
       <c r="Q7" s="6" t="n">
-        <v>6.278414617755686</v>
+        <v>3.574093053293836</v>
       </c>
       <c r="R7" s="6" t="n">
         <v>0</v>
       </c>
       <c r="S7" s="6" t="n">
-        <v>1.51e-06</v>
+        <v>4.81e-05</v>
       </c>
       <c r="T7" s="6" t="n">
-        <v>0.4</v>
+        <v>1.1</v>
       </c>
       <c r="U7" s="7" t="inlineStr">
         <is>
-          <t>GTCTTCCGATCTCTCCATACTCAAACCACCAGGAGGATGGACGACGGAGGAAGAAGAAGGAGCGGTGAGGAGGGTGAAGGTGAGGATTCCCAAAGCTGAGC</t>
+          <t>CTAATCCGCCGAGTCAAACCTAAGACGATCGTCGAAGTCGGGAGTTTTCTCGGCGCGTCGGCGATACACATGGCGAATCTCACGCGCCGACTTGGGCTCGAGGAGACTCAGATTCTATGCGTCGACGA</t>
         </is>
       </c>
       <c r="V7" s="6" t="n">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="W7" s="6" t="n">
-        <v>55.44554455445545</v>
+        <v>57.03125</v>
       </c>
       <c r="X7" s="6" t="n">
-        <v>-4.261404037475586</v>
-      </c>
-      <c r="Y7" s="6" t="inlineStr">
-        <is>
-          <t>CP002685.1</t>
-        </is>
-      </c>
+        <v>-13.85025310516357</v>
+      </c>
+      <c r="Y7" s="6" t="inlineStr"/>
       <c r="Z7" s="6" t="inlineStr">
         <is>
-          <t>164431</t>
+          <t>14</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>At17.1</t>
+          <t>CP002684.1</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>CATACTCAAACCACCAGGAG</t>
+          <t>GAACGATCCCGATACCATC</t>
         </is>
       </c>
       <c r="C8" s="6" t="n">
-        <v>57.70701631138252</v>
+        <v>57.18013716608459</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>1.457016311382517</v>
+        <v>1.385652307599617</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>-0.7797346115112305</v>
+        <v>-0.8097348213195801</v>
       </c>
       <c r="F8" s="6" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="G8" s="6" t="n">
-        <v>1.1</v>
-      </c>
+        <v>0.007</v>
+      </c>
+      <c r="G8" s="6" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr">
         <is>
-          <t>GGTGGCTCCTTCTTTAACG</t>
+          <t>CACATCCATACGCTAGGTG</t>
         </is>
       </c>
       <c r="I8" s="6" t="n">
-        <v>58.14276553363504</v>
+        <v>57.40147050241876</v>
       </c>
       <c r="J8" s="6" t="n">
-        <v>1.708555007319251</v>
+        <v>1.164318971265448</v>
       </c>
       <c r="K8" s="6" t="n">
         <v>0</v>
@@ -1183,183 +1160,175 @@
         <v>3.7</v>
       </c>
       <c r="N8" s="6" t="n">
-        <v>3.165571318701769</v>
+        <v>2.549971278865065</v>
       </c>
       <c r="O8" s="7" t="inlineStr">
         <is>
-          <t>TCCTCACCTTCACCCTCCTCACCGCT</t>
+          <t>TCGAGACCCAAAACACTCGCCGCAGT</t>
         </is>
       </c>
       <c r="P8" s="6" t="n">
-        <v>64.17251465903956</v>
+        <v>64.30135325099201</v>
       </c>
       <c r="Q8" s="6" t="n">
-        <v>6.827485340960436</v>
+        <v>6.698646749007992</v>
       </c>
       <c r="R8" s="6" t="n">
-        <v>0</v>
+        <v>-1.419864654541016</v>
       </c>
       <c r="S8" s="6" t="n">
         <v>1.51e-06</v>
       </c>
       <c r="T8" s="6" t="n">
-        <v>0.033</v>
+        <v>1.4</v>
       </c>
       <c r="U8" s="7" t="inlineStr">
         <is>
-          <t>CATACTCAAACCACCAGGAGGATGGACGACGGAGGAAGAAGAAGGAGCGGTGAGGAGGGTGAAGGTGAGGATTCCCAAAGCTGAGCTTGAAAAGCTCGTTAAAGAAGGAGCCACCG</t>
+          <t>GAACGATCCCGATACCATCCGTGAGATTCTTTTGCGGCAGGACGATGTTTTTTCATCGAGACCCAAAACACTCGCCGCAGTCCACCTAGCGTATGGATGTGG</t>
         </is>
       </c>
       <c r="V8" s="6" t="n">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="W8" s="6" t="n">
-        <v>53.44827586206896</v>
+        <v>51.9607843137255</v>
       </c>
       <c r="X8" s="6" t="n">
-        <v>-5.429211139678955</v>
-      </c>
-      <c r="Y8" s="6" t="inlineStr">
-        <is>
-          <t>CP002685.1</t>
-        </is>
-      </c>
+        <v>-5.947404861450195</v>
+      </c>
+      <c r="Y8" s="6" t="inlineStr"/>
       <c r="Z8" s="6" t="inlineStr">
         <is>
-          <t>164446</t>
+          <t>45</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>MTO1</t>
+          <t>CP002684.1</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>CTGGTGGATCTAGGAGGTAC</t>
+          <t>CAACGAACGATCCCGATAC</t>
         </is>
       </c>
       <c r="C9" s="6" t="n">
-        <v>58.11536079407438</v>
+        <v>58.1158368244387</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v>1.865360794074377</v>
+        <v>1.681626298122911</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>0</v>
+        <v>-0.8097348213195801</v>
       </c>
       <c r="F9" s="6" t="n">
-        <v>0.002</v>
+        <v>0.007</v>
       </c>
       <c r="G9" s="6" t="n">
-        <v>0.3</v>
+        <v>3.7</v>
       </c>
       <c r="H9" s="7" t="inlineStr">
         <is>
-          <t>GGGATCAGGGAGAAGATAGG</t>
+          <t>ATCCATACGCTAGGTGGAC</t>
         </is>
       </c>
       <c r="I9" s="6" t="n">
-        <v>58.1693460818891</v>
+        <v>58.25082796726878</v>
       </c>
       <c r="J9" s="6" t="n">
-        <v>1.919346081889103</v>
+        <v>1.816617440952985</v>
       </c>
       <c r="K9" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L9" s="6" t="n">
-        <v>0.002</v>
+        <v>0.007</v>
       </c>
       <c r="M9" s="6" t="n">
         <v>1.1</v>
       </c>
       <c r="N9" s="6" t="n">
-        <v>3.784706875963479</v>
+        <v>3.498243739075896</v>
       </c>
       <c r="O9" s="7" t="inlineStr">
         <is>
-          <t>CCGATGGGAGCCTCACTGTTCATGCCG</t>
+          <t>TCATCGAGACCCAAAACACTCGCCGCA</t>
         </is>
       </c>
       <c r="P9" s="6" t="n">
-        <v>64.81452393084095</v>
+        <v>64.20487603053124</v>
       </c>
       <c r="Q9" s="6" t="n">
-        <v>7.185476069159051</v>
+        <v>7.795123969468762</v>
       </c>
       <c r="R9" s="6" t="n">
-        <v>0</v>
+        <v>-1.419864654541016</v>
       </c>
       <c r="S9" s="6" t="n">
         <v>5.4e-07</v>
       </c>
       <c r="T9" s="6" t="n">
-        <v>0.51</v>
+        <v>0.042</v>
       </c>
       <c r="U9" s="7" t="inlineStr">
         <is>
-          <t>CTGGTGGATCTAGGAGGTACCGGCATGAACAGTGAGGCTCCCATCGGAGCTCAAGAAAGAATGTTTGGAATCCGTCAGCTGTACACTACCTATCTTCTCCCTGATCCCC</t>
+          <t>CAACGAACGATCCCGATACCATCCGTGAGATTCTTTTGCGGCAGGACGATGTTTTTTCATCGAGACCCAAAACACTCGCCGCAGTCCACCTAGCGTATGGATG</t>
         </is>
       </c>
       <c r="V9" s="6" t="n">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="W9" s="6" t="n">
-        <v>52.29357798165137</v>
+        <v>51.45631067961165</v>
       </c>
       <c r="X9" s="6" t="n">
-        <v>-3.461651563644409</v>
-      </c>
-      <c r="Y9" s="6" t="inlineStr">
-        <is>
-          <t>CP002686.1</t>
-        </is>
-      </c>
+        <v>-5.947404861450195</v>
+      </c>
+      <c r="Y9" s="6" t="inlineStr"/>
       <c r="Z9" s="6" t="inlineStr">
         <is>
-          <t>41300</t>
+          <t>41</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>MTO1</t>
+          <t>CP002685.1</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>CTGAATCTGGTGGATCTAGG</t>
+          <t>TCCGTCGACAGAGTCAATC</t>
         </is>
       </c>
       <c r="C10" s="6" t="n">
-        <v>56.59552606387956</v>
+        <v>58.81843131961955</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>2.154473936120439</v>
+        <v>2.384220793303758</v>
       </c>
       <c r="E10" s="6" t="n">
         <v>0</v>
       </c>
       <c r="F10" s="6" t="n">
-        <v>0.002</v>
+        <v>0.007</v>
       </c>
       <c r="G10" s="6" t="n">
-        <v>1.1</v>
+        <v>3.7</v>
       </c>
       <c r="H10" s="7" t="inlineStr">
         <is>
-          <t>CAGGGAGAAGATAGGTAGTG</t>
+          <t>TCATGACTCGGATCTTAGCC</t>
         </is>
       </c>
       <c r="I10" s="6" t="n">
-        <v>55.9357109944566</v>
+        <v>58.78643594651186</v>
       </c>
       <c r="J10" s="6" t="n">
-        <v>2.814289005543401</v>
+        <v>2.536435946511858</v>
       </c>
       <c r="K10" s="6" t="n">
         <v>0</v>
@@ -1371,89 +1340,85 @@
         <v>3.7</v>
       </c>
       <c r="N10" s="6" t="n">
-        <v>4.96876294166384</v>
+        <v>4.920656739815616</v>
       </c>
       <c r="O10" s="7" t="inlineStr">
         <is>
-          <t>CCGATGGGAGCCTCACTGTTCATGCCG</t>
+          <t>TGCAAGCCCACGCCGCCGAT</t>
         </is>
       </c>
       <c r="P10" s="6" t="n">
-        <v>64.81452393084095</v>
+        <v>64.4500508334425</v>
       </c>
       <c r="Q10" s="6" t="n">
-        <v>7.185476069159051</v>
+        <v>0.5499491665574965</v>
       </c>
       <c r="R10" s="6" t="n">
-        <v>0</v>
+        <v>-0.7097349166870117</v>
       </c>
       <c r="S10" s="6" t="n">
-        <v>5.4e-07</v>
+        <v>0.002</v>
       </c>
       <c r="T10" s="6" t="n">
-        <v>0.51</v>
+        <v>0.3</v>
       </c>
       <c r="U10" s="7" t="inlineStr">
         <is>
-          <t>CTGAATCTGGTGGATCTAGGAGGTACCGGCATGAACAGTGAGGCTCCCATCGGAGCTCAAGAAAGAATGTTTGGAATCCGTCAGCTGTACACTACCTATCTTCTCCCTGA</t>
+          <t>TCCGTCGACAGAGTCAATCTTATGCAAGCCCACGCCGCCGATCTCGTCAGAGATGCTTCCTTGAACGACCGAGTGGAGCTCACAGTCCGCGGAGACGTGGGGGCTAAGATCCGAGTCATGAA</t>
         </is>
       </c>
       <c r="V10" s="6" t="n">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="W10" s="6" t="n">
-        <v>50</v>
+        <v>57.37704918032787</v>
       </c>
       <c r="X10" s="6" t="n">
-        <v>-3.461651563644409</v>
-      </c>
-      <c r="Y10" s="6" t="inlineStr">
-        <is>
-          <t>CP002686.1</t>
-        </is>
-      </c>
+        <v>-5.358549118041992</v>
+      </c>
+      <c r="Y10" s="6" t="inlineStr"/>
       <c r="Z10" s="6" t="inlineStr">
         <is>
-          <t>41294</t>
+          <t>8</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>XSP1</t>
+          <t>CP002685.1</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
         <is>
-          <t>CTACGACATGGACGACATC</t>
+          <t>GTCTTCCGATCTCTCCATAC</t>
         </is>
       </c>
       <c r="C11" s="6" t="n">
-        <v>57.44369071181501</v>
+        <v>56.72627428247569</v>
       </c>
       <c r="D11" s="6" t="n">
-        <v>1.1220987618692</v>
+        <v>2.023725717524314</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>-0.3097348213195801</v>
+        <v>0</v>
       </c>
       <c r="F11" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="G11" s="6" t="n">
-        <v>1.1</v>
+        <v>0.3</v>
       </c>
       <c r="H11" s="7" t="inlineStr">
         <is>
-          <t>GACAATGGAGGAACAGCTC</t>
+          <t>CTCAGCTTTGGGAATCCTC</t>
         </is>
       </c>
       <c r="I11" s="6" t="n">
-        <v>57.83082272420569</v>
+        <v>57.50429449531657</v>
       </c>
       <c r="J11" s="6" t="n">
-        <v>1.396612197889898</v>
+        <v>1.07008396900078</v>
       </c>
       <c r="K11" s="6" t="n">
         <v>0</v>
@@ -1465,89 +1430,85 @@
         <v>1.1</v>
       </c>
       <c r="N11" s="6" t="n">
-        <v>2.518710959759098</v>
+        <v>3.093809686525095</v>
       </c>
       <c r="O11" s="7" t="inlineStr">
         <is>
-          <t>AGCTCCATTGGTGGGTACACGCTCCG</t>
+          <t>CCTCCGTCGTCCATCCTCCTGGTGGT</t>
         </is>
       </c>
       <c r="P11" s="6" t="n">
-        <v>64.22598535419934</v>
+        <v>64.72158538224431</v>
       </c>
       <c r="Q11" s="6" t="n">
-        <v>6.774014645800662</v>
+        <v>6.278414617755686</v>
       </c>
       <c r="R11" s="6" t="n">
-        <v>-0.7341697216033936</v>
+        <v>0</v>
       </c>
       <c r="S11" s="6" t="n">
         <v>1.51e-06</v>
       </c>
       <c r="T11" s="6" t="n">
-        <v>1.4</v>
+        <v>0.4</v>
       </c>
       <c r="U11" s="7" t="inlineStr">
         <is>
-          <t>CTACGACATGGACGACATCTCCTATGTTCAGTTCTTGTGCGGCGAAGGCTACAACGCAACCACTCTAGCTCCATTGGTGGGTACACGCTCCGTGAGCTGTTCCTCCATTGTCC</t>
+          <t>GTCTTCCGATCTCTCCATACTCAAACCACCAGGAGGATGGACGACGGAGGAAGAAGAAGGAGCGGTGAGGAGGGTGAAGGTGAGGATTCCCAAAGCTGAGC</t>
         </is>
       </c>
       <c r="V11" s="6" t="n">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="W11" s="6" t="n">
-        <v>53.98230088495575</v>
+        <v>55.44554455445545</v>
       </c>
       <c r="X11" s="6" t="n">
-        <v>-6.521465301513672</v>
-      </c>
-      <c r="Y11" s="6" t="inlineStr">
-        <is>
-          <t>CP002687.1</t>
-        </is>
-      </c>
+        <v>-4.261404037475586</v>
+      </c>
+      <c r="Y11" s="6" t="inlineStr"/>
       <c r="Z11" s="6" t="inlineStr">
         <is>
-          <t>96840</t>
+          <t>10</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>XSP1</t>
+          <t>CP002685.1</t>
         </is>
       </c>
       <c r="B12" s="7" t="inlineStr">
         <is>
-          <t>CTGGCTTAGTCTACGACATG</t>
+          <t>CATACTCAAACCACCAGGAG</t>
         </is>
       </c>
       <c r="C12" s="6" t="n">
-        <v>57.6139686963578</v>
+        <v>57.70701631138252</v>
       </c>
       <c r="D12" s="6" t="n">
-        <v>1.363968696357801</v>
+        <v>1.457016311382517</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>0</v>
+        <v>-0.7797346115112305</v>
       </c>
       <c r="F12" s="6" t="n">
         <v>0.002</v>
       </c>
       <c r="G12" s="6" t="n">
-        <v>3.7</v>
+        <v>1.1</v>
       </c>
       <c r="H12" s="7" t="inlineStr">
         <is>
-          <t>AGGGACAATGGAGGAACAG</t>
+          <t>GGTGGCTCCTTCTTTAACG</t>
         </is>
       </c>
       <c r="I12" s="6" t="n">
-        <v>58.60725372965351</v>
+        <v>58.14276553363504</v>
       </c>
       <c r="J12" s="6" t="n">
-        <v>2.173043203337716</v>
+        <v>1.708555007319251</v>
       </c>
       <c r="K12" s="6" t="n">
         <v>0</v>
@@ -1556,92 +1517,88 @@
         <v>0.007</v>
       </c>
       <c r="M12" s="6" t="n">
-        <v>1.1</v>
+        <v>3.7</v>
       </c>
       <c r="N12" s="6" t="n">
-        <v>3.537011899695518</v>
+        <v>3.165571318701769</v>
       </c>
       <c r="O12" s="7" t="inlineStr">
         <is>
-          <t>AGCTCCATTGGTGGGTACACGCTCCG</t>
+          <t>TCCTCACCTTCACCCTCCTCACCGCT</t>
         </is>
       </c>
       <c r="P12" s="6" t="n">
-        <v>64.22598535419934</v>
+        <v>64.17251465903956</v>
       </c>
       <c r="Q12" s="6" t="n">
-        <v>6.774014645800662</v>
+        <v>6.827485340960436</v>
       </c>
       <c r="R12" s="6" t="n">
-        <v>-0.7341697216033936</v>
+        <v>0</v>
       </c>
       <c r="S12" s="6" t="n">
         <v>1.51e-06</v>
       </c>
       <c r="T12" s="6" t="n">
-        <v>1.4</v>
+        <v>0.033</v>
       </c>
       <c r="U12" s="7" t="inlineStr">
         <is>
-          <t>CTGGCTTAGTCTACGACATGGACGACATCTCCTATGTTCAGTTCTTGTGCGGCGAAGGCTACAACGCAACCACTCTAGCTCCATTGGTGGGTACACGCTCCGTGAGCTGTTCCTCCATTGTCCCTG</t>
+          <t>CATACTCAAACCACCAGGAGGATGGACGACGGAGGAAGAAGAAGGAGCGGTGAGGAGGGTGAAGGTGAGGATTCCCAAAGCTGAGCTTGAAAAGCTCGTTAAAGAAGGAGCCACCG</t>
         </is>
       </c>
       <c r="V12" s="6" t="n">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="W12" s="6" t="n">
-        <v>53.96825396825397</v>
+        <v>53.44827586206896</v>
       </c>
       <c r="X12" s="6" t="n">
-        <v>-6.521465301513672</v>
-      </c>
-      <c r="Y12" s="6" t="inlineStr">
-        <is>
-          <t>CP002687.1</t>
-        </is>
-      </c>
+        <v>-5.429211139678955</v>
+      </c>
+      <c r="Y12" s="6" t="inlineStr"/>
       <c r="Z12" s="6" t="inlineStr">
         <is>
-          <t>96830</t>
+          <t>25</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="inlineStr">
         <is>
-          <t>XSP1</t>
+          <t>CP002686.1</t>
         </is>
       </c>
       <c r="B13" s="7" t="inlineStr">
         <is>
-          <t>CCCAACAATCCAACTCACG</t>
+          <t>CTGGTGGATCTAGGAGGTAC</t>
         </is>
       </c>
       <c r="C13" s="6" t="n">
-        <v>58.74250943646473</v>
+        <v>58.11536079407438</v>
       </c>
       <c r="D13" s="6" t="n">
-        <v>2.308298910148938</v>
+        <v>1.865360794074377</v>
       </c>
       <c r="E13" s="6" t="n">
         <v>0</v>
       </c>
       <c r="F13" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="G13" s="6" t="n">
-        <v>3.7</v>
+        <v>0.3</v>
       </c>
       <c r="H13" s="7" t="inlineStr">
         <is>
-          <t>CCACCACTTTGAAGCTTCTC</t>
+          <t>GGGATCAGGGAGAAGATAGG</t>
         </is>
       </c>
       <c r="I13" s="6" t="n">
-        <v>58.87532172899461</v>
+        <v>58.1693460818891</v>
       </c>
       <c r="J13" s="6" t="n">
-        <v>2.625321728994606</v>
+        <v>1.919346081889103</v>
       </c>
       <c r="K13" s="6" t="n">
         <v>0</v>
@@ -1650,164 +1607,158 @@
         <v>0.002</v>
       </c>
       <c r="M13" s="6" t="n">
-        <v>0.3</v>
+        <v>1.1</v>
       </c>
       <c r="N13" s="6" t="n">
-        <v>4.933620639143545</v>
+        <v>3.784706875963479</v>
       </c>
       <c r="O13" s="7" t="inlineStr">
         <is>
-          <t>CCGCCACCGTCCGAGCACCG</t>
+          <t>CCGATGGGAGCCTCACTGTTCATGCCG</t>
         </is>
       </c>
       <c r="P13" s="6" t="n">
-        <v>64.7335341111355</v>
+        <v>64.81452393084095</v>
       </c>
       <c r="Q13" s="6" t="n">
-        <v>0.2664658888645022</v>
+        <v>7.185476069159051</v>
       </c>
       <c r="R13" s="6" t="n">
         <v>0</v>
       </c>
       <c r="S13" s="6" t="n">
-        <v>0.002</v>
+        <v>5.4e-07</v>
       </c>
       <c r="T13" s="6" t="n">
-        <v>1.1</v>
+        <v>0.51</v>
       </c>
       <c r="U13" s="7" t="inlineStr">
         <is>
-          <t>CCCAACAATCCAACTCACGTTGAGATCCGCCAAAACGTCCACATTGGCTGTGTTCAGGCGGAGAGTCACCAACGTGGGACCACCGTCGTCGGTCTACACCGCCACCGTCCGAGCACCGAAAGGAGTAGAAATCACGGTGGAGCCACAGAGTTTGTCATTTTCAAAGGCTTCACAAAAGAGAAGCTTCAAAGTGGTGGT</t>
+          <t>CTGGTGGATCTAGGAGGTACCGGCATGAACAGTGAGGCTCCCATCGGAGCTCAAGAAAGAATGTTTGGAATCCGTCAGCTGTACACTACCTATCTTCTCCCTGATCCCC</t>
         </is>
       </c>
       <c r="V13" s="6" t="n">
-        <v>197</v>
+        <v>108</v>
       </c>
       <c r="W13" s="6" t="n">
-        <v>53.03030303030303</v>
+        <v>52.29357798165137</v>
       </c>
       <c r="X13" s="6" t="n">
-        <v>-17.26604652404785</v>
-      </c>
-      <c r="Y13" s="6" t="inlineStr">
-        <is>
-          <t>CP002687.1</t>
-        </is>
-      </c>
+        <v>-3.461651563644409</v>
+      </c>
+      <c r="Y13" s="6" t="inlineStr"/>
       <c r="Z13" s="6" t="inlineStr">
         <is>
-          <t>96981</t>
+          <t>72</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
         <is>
-          <t>RLK4</t>
+          <t>CP002686.1</t>
         </is>
       </c>
       <c r="B14" s="7" t="inlineStr">
         <is>
-          <t>GAGCTGGAACATGTTCTGG</t>
+          <t>CTGAATCTGGTGGATCTAGG</t>
         </is>
       </c>
       <c r="C14" s="6" t="n">
-        <v>58.13313451624401</v>
+        <v>56.59552606387956</v>
       </c>
       <c r="D14" s="6" t="n">
-        <v>1.698923989928222</v>
+        <v>2.154473936120439</v>
       </c>
       <c r="E14" s="6" t="n">
         <v>0</v>
       </c>
       <c r="F14" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="G14" s="6" t="n">
         <v>1.1</v>
       </c>
       <c r="H14" s="7" t="inlineStr">
         <is>
-          <t>CACAGGGCTTGAGCAATTC</t>
+          <t>CAGGGAGAAGATAGGTAGTG</t>
         </is>
       </c>
       <c r="I14" s="6" t="n">
-        <v>59.11187222956136</v>
+        <v>55.9357109944566</v>
       </c>
       <c r="J14" s="6" t="n">
-        <v>2.677661703245565</v>
+        <v>2.814289005543401</v>
       </c>
       <c r="K14" s="6" t="n">
-        <v>-0.790266752243042</v>
+        <v>0</v>
       </c>
       <c r="L14" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="M14" s="6" t="n">
         <v>3.7</v>
       </c>
       <c r="N14" s="6" t="n">
-        <v>4.376585693173787</v>
+        <v>4.96876294166384</v>
       </c>
       <c r="O14" s="7" t="inlineStr">
         <is>
-          <t>ACGCGGCAAGGATCCTCCGGCT</t>
+          <t>CCGATGGGAGCCTCACTGTTCATGCCG</t>
         </is>
       </c>
       <c r="P14" s="6" t="n">
-        <v>64.70494890469467</v>
+        <v>64.81452393084095</v>
       </c>
       <c r="Q14" s="6" t="n">
-        <v>2.295051095305325</v>
+        <v>7.185476069159051</v>
       </c>
       <c r="R14" s="6" t="n">
-        <v>-0.9579751491546631</v>
+        <v>0</v>
       </c>
       <c r="S14" s="6" t="n">
-        <v>0.000168</v>
-      </c>
-      <c r="T14" s="6" t="inlineStr"/>
+        <v>5.4e-07</v>
+      </c>
+      <c r="T14" s="6" t="n">
+        <v>0.51</v>
+      </c>
       <c r="U14" s="7" t="inlineStr">
         <is>
-          <t>GAGCTGGAACATGTTCTGGTTGCAGCCGGAGGATCCTTGCCGCGTTTACAATCTCTGTGGTCAATTAGGGTTTTGTAGCAGCGAATTGCTCAAGCCCTGTGC</t>
+          <t>CTGAATCTGGTGGATCTAGGAGGTACCGGCATGAACAGTGAGGCTCCCATCGGAGCTCAAGAAAGAATGTTTGGAATCCGTCAGCTGTACACTACCTATCTTCTCCCTGA</t>
         </is>
       </c>
       <c r="V14" s="6" t="n">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="W14" s="6" t="n">
-        <v>51.9607843137255</v>
+        <v>50</v>
       </c>
       <c r="X14" s="6" t="n">
-        <v>-6.424409866333008</v>
-      </c>
-      <c r="Y14" s="6" t="inlineStr">
-        <is>
-          <t>CP002687.1</t>
-        </is>
-      </c>
+        <v>-3.461651563644409</v>
+      </c>
+      <c r="Y14" s="6" t="inlineStr"/>
       <c r="Z14" s="6" t="inlineStr">
         <is>
-          <t>149753</t>
+          <t>66</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="6" t="inlineStr">
         <is>
-          <t>CYP86A2</t>
+          <t>CP002686.1</t>
         </is>
       </c>
       <c r="B15" s="7" t="inlineStr">
         <is>
-          <t>GTATGCACGACTGGATCAC</t>
+          <t>CTTGAGACTGAGGAATGCG</t>
         </is>
       </c>
       <c r="C15" s="6" t="n">
-        <v>58.01929187670885</v>
+        <v>57.93566240021704</v>
       </c>
       <c r="D15" s="6" t="n">
-        <v>1.585081350393057</v>
+        <v>1.501451873901249</v>
       </c>
       <c r="E15" s="6" t="n">
         <v>0</v>
@@ -1820,69 +1771,65 @@
       </c>
       <c r="H15" s="7" t="inlineStr">
         <is>
-          <t>GTAGTTGTCGAACCTGGTC</t>
+          <t>CCTTACAGAACAACCACACC</t>
         </is>
       </c>
       <c r="I15" s="6" t="n">
-        <v>57.48615986233125</v>
+        <v>58.51220659203409</v>
       </c>
       <c r="J15" s="6" t="n">
-        <v>1.07962961135296</v>
+        <v>2.26220659203409</v>
       </c>
       <c r="K15" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L15" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="M15" s="6" t="n">
         <v>1.1</v>
       </c>
       <c r="N15" s="6" t="n">
-        <v>2.664710961746017</v>
+        <v>3.76365846593534</v>
       </c>
       <c r="O15" s="7" t="inlineStr">
         <is>
-          <t>GCCGCCACACGCACGGAGGT</t>
+          <t>GCTCTGAAAACAAGCACGGCTCGCCCA</t>
         </is>
       </c>
       <c r="P15" s="6" t="n">
-        <v>64.65986280657165</v>
+        <v>65.50373796818639</v>
       </c>
       <c r="Q15" s="6" t="n">
-        <v>0.3401371934283475</v>
+        <v>7.503737968186385</v>
       </c>
       <c r="R15" s="6" t="n">
-        <v>-1.617270469665527</v>
+        <v>0</v>
       </c>
       <c r="S15" s="6" t="n">
-        <v>0.002</v>
+        <v>5.4e-07</v>
       </c>
       <c r="T15" s="6" t="n">
-        <v>1.1</v>
+        <v>0.001</v>
       </c>
       <c r="U15" s="7" t="inlineStr">
         <is>
-          <t>GTATGCACGACTGGATCACTGAGAACCTCCGTGCGTGTGGCGGCACTTATCAGACATGTATCTGCGCCGTACCTTTCTTGGCAAAAAAGCAAGGTCTCGTGACCGTCACGTGCGATCCCAAGAACATCGAACACATGCTCAAGACCAGGTTCGACAACTACC</t>
+          <t>CTTGAGACTGAGGAATGCGTCAAGAGCTCCAGCAACAAGAGGGGAATGTTTGAGTTGCCTCGTGTTCATCACCGTGAATTGGAAGCTGAGCTGAAGAAGATGGCTCCGCCTAATGGGCGAGCCGTGCTTGTTTTCAGAGCGAGGTGTGGTTGTTCTGTAAGGA</t>
         </is>
       </c>
       <c r="V15" s="6" t="n">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="W15" s="6" t="n">
-        <v>52.46913580246913</v>
+        <v>51.53374233128834</v>
       </c>
       <c r="X15" s="6" t="n">
-        <v>-10.59030723571777</v>
-      </c>
-      <c r="Y15" s="6" t="inlineStr">
-        <is>
-          <t>CP002687.1</t>
-        </is>
-      </c>
+        <v>-7.891154766082764</v>
+      </c>
+      <c r="Y15" s="6" t="inlineStr"/>
       <c r="Z15" s="6" t="inlineStr">
         <is>
-          <t>161094</t>
+          <t>31</t>
         </is>
       </c>
     </row>
@@ -1892,179 +1839,537 @@
           <t>CP002687.1</t>
         </is>
       </c>
-      <c r="B16" s="8" t="inlineStr">
-        <is>
-          <t>No suitable primers found</t>
-        </is>
-      </c>
-      <c r="C16" s="6" t="inlineStr"/>
-      <c r="D16" s="6" t="inlineStr"/>
-      <c r="E16" s="6" t="inlineStr"/>
-      <c r="F16" s="6" t="inlineStr"/>
-      <c r="G16" s="6" t="inlineStr"/>
-      <c r="H16" s="7" t="inlineStr"/>
-      <c r="I16" s="6" t="inlineStr"/>
-      <c r="J16" s="6" t="inlineStr"/>
-      <c r="K16" s="6" t="inlineStr"/>
-      <c r="L16" s="6" t="inlineStr"/>
-      <c r="M16" s="6" t="inlineStr"/>
-      <c r="N16" s="6" t="inlineStr"/>
-      <c r="O16" s="7" t="inlineStr"/>
-      <c r="P16" s="6" t="inlineStr"/>
-      <c r="Q16" s="6" t="inlineStr"/>
-      <c r="R16" s="6" t="inlineStr"/>
-      <c r="S16" s="6" t="inlineStr"/>
-      <c r="T16" s="6" t="inlineStr"/>
-      <c r="U16" s="7" t="inlineStr"/>
-      <c r="V16" s="6" t="inlineStr"/>
-      <c r="W16" s="6" t="inlineStr"/>
-      <c r="X16" s="6" t="inlineStr"/>
+      <c r="B16" s="7" t="inlineStr">
+        <is>
+          <t>CCTAGAGTACACCGGTTCTC</t>
+        </is>
+      </c>
+      <c r="C16" s="6" t="n">
+        <v>58.72687468691566</v>
+      </c>
+      <c r="D16" s="6" t="n">
+        <v>2.476874686915664</v>
+      </c>
+      <c r="E16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="6" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="G16" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H16" s="7" t="inlineStr">
+        <is>
+          <t>GAGACTCATTGGTTCGTGTC</t>
+        </is>
+      </c>
+      <c r="I16" s="6" t="n">
+        <v>58.3997252290801</v>
+      </c>
+      <c r="J16" s="6" t="n">
+        <v>2.149725229080104</v>
+      </c>
+      <c r="K16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="6" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="M16" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="N16" s="6" t="n">
+        <v>4.626599915995769</v>
+      </c>
+      <c r="O16" s="7" t="inlineStr">
+        <is>
+          <t>CGCGCCAGAATCAAGCCTCCTTCACG</t>
+        </is>
+      </c>
+      <c r="P16" s="6" t="n">
+        <v>64.0105612867751</v>
+      </c>
+      <c r="Q16" s="6" t="n">
+        <v>6.989438713224899</v>
+      </c>
+      <c r="R16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" s="6" t="n">
+        <v>1.51e-06</v>
+      </c>
+      <c r="T16" s="6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="U16" s="7" t="inlineStr">
+        <is>
+          <t>CCTAGAGTACACCGGTTCTCCACAACTTGGGTGGAATCTTGAGCGTGAAGGAGGCTTGATTCTGGCGCGAGACACGAACCAATGAGTCTCA</t>
+        </is>
+      </c>
+      <c r="V16" s="6" t="n">
+        <v>90</v>
+      </c>
+      <c r="W16" s="6" t="n">
+        <v>52.74725274725275</v>
+      </c>
+      <c r="X16" s="6" t="n">
+        <v>-4.578721046447754</v>
+      </c>
       <c r="Y16" s="6" t="inlineStr"/>
-      <c r="Z16" s="6" t="inlineStr"/>
+      <c r="Z16" s="6" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="inlineStr">
         <is>
-          <t>CP002684.1</t>
-        </is>
-      </c>
-      <c r="B17" s="8" t="inlineStr">
-        <is>
-          <t>No suitable primers found</t>
-        </is>
-      </c>
-      <c r="C17" s="6" t="inlineStr"/>
-      <c r="D17" s="6" t="inlineStr"/>
-      <c r="E17" s="6" t="inlineStr"/>
-      <c r="F17" s="6" t="inlineStr"/>
-      <c r="G17" s="6" t="inlineStr"/>
-      <c r="H17" s="7" t="inlineStr"/>
-      <c r="I17" s="6" t="inlineStr"/>
-      <c r="J17" s="6" t="inlineStr"/>
-      <c r="K17" s="6" t="inlineStr"/>
-      <c r="L17" s="6" t="inlineStr"/>
-      <c r="M17" s="6" t="inlineStr"/>
-      <c r="N17" s="6" t="inlineStr"/>
-      <c r="O17" s="7" t="inlineStr"/>
-      <c r="P17" s="6" t="inlineStr"/>
-      <c r="Q17" s="6" t="inlineStr"/>
-      <c r="R17" s="6" t="inlineStr"/>
-      <c r="S17" s="6" t="inlineStr"/>
-      <c r="T17" s="6" t="inlineStr"/>
-      <c r="U17" s="7" t="inlineStr"/>
-      <c r="V17" s="6" t="inlineStr"/>
-      <c r="W17" s="6" t="inlineStr"/>
-      <c r="X17" s="6" t="inlineStr"/>
+          <t>CP002687.1</t>
+        </is>
+      </c>
+      <c r="B17" s="7" t="inlineStr">
+        <is>
+          <t>CTACGACATGGACGACATC</t>
+        </is>
+      </c>
+      <c r="C17" s="6" t="n">
+        <v>57.44369071181501</v>
+      </c>
+      <c r="D17" s="6" t="n">
+        <v>1.1220987618692</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>-0.3097348213195801</v>
+      </c>
+      <c r="F17" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H17" s="7" t="inlineStr">
+        <is>
+          <t>GACAATGGAGGAACAGCTC</t>
+        </is>
+      </c>
+      <c r="I17" s="6" t="n">
+        <v>57.83082272420569</v>
+      </c>
+      <c r="J17" s="6" t="n">
+        <v>1.396612197889898</v>
+      </c>
+      <c r="K17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="M17" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="N17" s="6" t="n">
+        <v>2.518710959759098</v>
+      </c>
+      <c r="O17" s="7" t="inlineStr">
+        <is>
+          <t>AGCTCCATTGGTGGGTACACGCTCCG</t>
+        </is>
+      </c>
+      <c r="P17" s="6" t="n">
+        <v>64.22598535419934</v>
+      </c>
+      <c r="Q17" s="6" t="n">
+        <v>6.774014645800662</v>
+      </c>
+      <c r="R17" s="6" t="n">
+        <v>-0.7341697216033936</v>
+      </c>
+      <c r="S17" s="6" t="n">
+        <v>1.51e-06</v>
+      </c>
+      <c r="T17" s="6" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="U17" s="7" t="inlineStr">
+        <is>
+          <t>CTACGACATGGACGACATCTCCTATGTTCAGTTCTTGTGCGGCGAAGGCTACAACGCAACCACTCTAGCTCCATTGGTGGGTACACGCTCCGTGAGCTGTTCCTCCATTGTCC</t>
+        </is>
+      </c>
+      <c r="V17" s="6" t="n">
+        <v>112</v>
+      </c>
+      <c r="W17" s="6" t="n">
+        <v>53.98230088495575</v>
+      </c>
+      <c r="X17" s="6" t="n">
+        <v>-6.521465301513672</v>
+      </c>
       <c r="Y17" s="6" t="inlineStr"/>
-      <c r="Z17" s="6" t="inlineStr"/>
+      <c r="Z17" s="6" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="inlineStr">
         <is>
-          <t>CP002688.1</t>
-        </is>
-      </c>
-      <c r="B18" s="8" t="inlineStr">
-        <is>
-          <t>No suitable primers found</t>
-        </is>
-      </c>
-      <c r="C18" s="6" t="inlineStr"/>
-      <c r="D18" s="6" t="inlineStr"/>
-      <c r="E18" s="6" t="inlineStr"/>
-      <c r="F18" s="6" t="inlineStr"/>
-      <c r="G18" s="6" t="inlineStr"/>
-      <c r="H18" s="7" t="inlineStr"/>
-      <c r="I18" s="6" t="inlineStr"/>
-      <c r="J18" s="6" t="inlineStr"/>
-      <c r="K18" s="6" t="inlineStr"/>
-      <c r="L18" s="6" t="inlineStr"/>
-      <c r="M18" s="6" t="inlineStr"/>
-      <c r="N18" s="6" t="inlineStr"/>
-      <c r="O18" s="7" t="inlineStr"/>
-      <c r="P18" s="6" t="inlineStr"/>
-      <c r="Q18" s="6" t="inlineStr"/>
-      <c r="R18" s="6" t="inlineStr"/>
-      <c r="S18" s="6" t="inlineStr"/>
-      <c r="T18" s="6" t="inlineStr"/>
-      <c r="U18" s="7" t="inlineStr"/>
-      <c r="V18" s="6" t="inlineStr"/>
-      <c r="W18" s="6" t="inlineStr"/>
-      <c r="X18" s="6" t="inlineStr"/>
+          <t>CP002687.1</t>
+        </is>
+      </c>
+      <c r="B18" s="7" t="inlineStr">
+        <is>
+          <t>CTGGCTTAGTCTACGACATG</t>
+        </is>
+      </c>
+      <c r="C18" s="6" t="n">
+        <v>57.6139686963578</v>
+      </c>
+      <c r="D18" s="6" t="n">
+        <v>1.363968696357801</v>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="6" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="G18" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H18" s="7" t="inlineStr">
+        <is>
+          <t>AGGGACAATGGAGGAACAG</t>
+        </is>
+      </c>
+      <c r="I18" s="6" t="n">
+        <v>58.60725372965351</v>
+      </c>
+      <c r="J18" s="6" t="n">
+        <v>2.173043203337716</v>
+      </c>
+      <c r="K18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="M18" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="N18" s="6" t="n">
+        <v>3.537011899695518</v>
+      </c>
+      <c r="O18" s="7" t="inlineStr">
+        <is>
+          <t>AGCTCCATTGGTGGGTACACGCTCCG</t>
+        </is>
+      </c>
+      <c r="P18" s="6" t="n">
+        <v>64.22598535419934</v>
+      </c>
+      <c r="Q18" s="6" t="n">
+        <v>6.774014645800662</v>
+      </c>
+      <c r="R18" s="6" t="n">
+        <v>-0.7341697216033936</v>
+      </c>
+      <c r="S18" s="6" t="n">
+        <v>1.51e-06</v>
+      </c>
+      <c r="T18" s="6" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="U18" s="7" t="inlineStr">
+        <is>
+          <t>CTGGCTTAGTCTACGACATGGACGACATCTCCTATGTTCAGTTCTTGTGCGGCGAAGGCTACAACGCAACCACTCTAGCTCCATTGGTGGGTACACGCTCCGTGAGCTGTTCCTCCATTGTCCCTG</t>
+        </is>
+      </c>
+      <c r="V18" s="6" t="n">
+        <v>125</v>
+      </c>
+      <c r="W18" s="6" t="n">
+        <v>53.96825396825397</v>
+      </c>
+      <c r="X18" s="6" t="n">
+        <v>-6.521465301513672</v>
+      </c>
       <c r="Y18" s="6" t="inlineStr"/>
-      <c r="Z18" s="6" t="inlineStr"/>
+      <c r="Z18" s="6" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="inlineStr">
         <is>
-          <t>CP002685.1</t>
-        </is>
-      </c>
-      <c r="B19" s="8" t="inlineStr">
-        <is>
-          <t>No suitable primers found</t>
-        </is>
-      </c>
-      <c r="C19" s="6" t="inlineStr"/>
-      <c r="D19" s="6" t="inlineStr"/>
-      <c r="E19" s="6" t="inlineStr"/>
-      <c r="F19" s="6" t="inlineStr"/>
-      <c r="G19" s="6" t="inlineStr"/>
-      <c r="H19" s="7" t="inlineStr"/>
-      <c r="I19" s="6" t="inlineStr"/>
-      <c r="J19" s="6" t="inlineStr"/>
-      <c r="K19" s="6" t="inlineStr"/>
-      <c r="L19" s="6" t="inlineStr"/>
-      <c r="M19" s="6" t="inlineStr"/>
-      <c r="N19" s="6" t="inlineStr"/>
-      <c r="O19" s="7" t="inlineStr"/>
-      <c r="P19" s="6" t="inlineStr"/>
-      <c r="Q19" s="6" t="inlineStr"/>
-      <c r="R19" s="6" t="inlineStr"/>
-      <c r="S19" s="6" t="inlineStr"/>
-      <c r="T19" s="6" t="inlineStr"/>
-      <c r="U19" s="7" t="inlineStr"/>
-      <c r="V19" s="6" t="inlineStr"/>
-      <c r="W19" s="6" t="inlineStr"/>
-      <c r="X19" s="6" t="inlineStr"/>
+          <t>CP002687.1</t>
+        </is>
+      </c>
+      <c r="B19" s="7" t="inlineStr">
+        <is>
+          <t>CCCAACAATCCAACTCACG</t>
+        </is>
+      </c>
+      <c r="C19" s="6" t="n">
+        <v>58.74250943646473</v>
+      </c>
+      <c r="D19" s="6" t="n">
+        <v>2.308298910148938</v>
+      </c>
+      <c r="E19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G19" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H19" s="7" t="inlineStr">
+        <is>
+          <t>CCACCACTTTGAAGCTTCTC</t>
+        </is>
+      </c>
+      <c r="I19" s="6" t="n">
+        <v>58.87532172899461</v>
+      </c>
+      <c r="J19" s="6" t="n">
+        <v>2.625321728994606</v>
+      </c>
+      <c r="K19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" s="6" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="M19" s="6" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="N19" s="6" t="n">
+        <v>4.933620639143545</v>
+      </c>
+      <c r="O19" s="7" t="inlineStr">
+        <is>
+          <t>CCGCCACCGTCCGAGCACCG</t>
+        </is>
+      </c>
+      <c r="P19" s="6" t="n">
+        <v>64.7335341111355</v>
+      </c>
+      <c r="Q19" s="6" t="n">
+        <v>0.2664658888645022</v>
+      </c>
+      <c r="R19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" s="6" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="T19" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="U19" s="7" t="inlineStr">
+        <is>
+          <t>CCCAACAATCCAACTCACGTTGAGATCCGCCAAAACGTCCACATTGGCTGTGTTCAGGCGGAGAGTCACCAACGTGGGACCACCGTCGTCGGTCTACACCGCCACCGTCCGAGCACCGAAAGGAGTAGAAATCACGGTGGAGCCACAGAGTTTGTCATTTTCAAAGGCTTCACAAAAGAGAAGCTTCAAAGTGGTGGT</t>
+        </is>
+      </c>
+      <c r="V19" s="6" t="n">
+        <v>197</v>
+      </c>
+      <c r="W19" s="6" t="n">
+        <v>53.03030303030303</v>
+      </c>
+      <c r="X19" s="6" t="n">
+        <v>-17.26604652404785</v>
+      </c>
       <c r="Y19" s="6" t="inlineStr"/>
-      <c r="Z19" s="6" t="inlineStr"/>
+      <c r="Z19" s="6" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="inlineStr">
         <is>
-          <t>CP002686.1</t>
-        </is>
-      </c>
-      <c r="B20" s="8" t="inlineStr">
-        <is>
-          <t>No suitable primers found</t>
-        </is>
-      </c>
-      <c r="C20" s="6" t="inlineStr"/>
-      <c r="D20" s="6" t="inlineStr"/>
-      <c r="E20" s="6" t="inlineStr"/>
-      <c r="F20" s="6" t="inlineStr"/>
-      <c r="G20" s="6" t="inlineStr"/>
-      <c r="H20" s="7" t="inlineStr"/>
-      <c r="I20" s="6" t="inlineStr"/>
-      <c r="J20" s="6" t="inlineStr"/>
-      <c r="K20" s="6" t="inlineStr"/>
-      <c r="L20" s="6" t="inlineStr"/>
-      <c r="M20" s="6" t="inlineStr"/>
-      <c r="N20" s="6" t="inlineStr"/>
-      <c r="O20" s="7" t="inlineStr"/>
-      <c r="P20" s="6" t="inlineStr"/>
-      <c r="Q20" s="6" t="inlineStr"/>
-      <c r="R20" s="6" t="inlineStr"/>
-      <c r="S20" s="6" t="inlineStr"/>
+          <t>CP002687.1</t>
+        </is>
+      </c>
+      <c r="B20" s="7" t="inlineStr">
+        <is>
+          <t>GAGCTGGAACATGTTCTGG</t>
+        </is>
+      </c>
+      <c r="C20" s="6" t="n">
+        <v>58.13313451624401</v>
+      </c>
+      <c r="D20" s="6" t="n">
+        <v>1.698923989928222</v>
+      </c>
+      <c r="E20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G20" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H20" s="7" t="inlineStr">
+        <is>
+          <t>CACAGGGCTTGAGCAATTC</t>
+        </is>
+      </c>
+      <c r="I20" s="6" t="n">
+        <v>59.11187222956136</v>
+      </c>
+      <c r="J20" s="6" t="n">
+        <v>2.677661703245565</v>
+      </c>
+      <c r="K20" s="6" t="n">
+        <v>-0.790266752243042</v>
+      </c>
+      <c r="L20" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="M20" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="N20" s="6" t="n">
+        <v>4.376585693173787</v>
+      </c>
+      <c r="O20" s="7" t="inlineStr">
+        <is>
+          <t>ACGCGGCAAGGATCCTCCGGCT</t>
+        </is>
+      </c>
+      <c r="P20" s="6" t="n">
+        <v>64.70494890469467</v>
+      </c>
+      <c r="Q20" s="6" t="n">
+        <v>2.295051095305325</v>
+      </c>
+      <c r="R20" s="6" t="n">
+        <v>-0.9579751491546631</v>
+      </c>
+      <c r="S20" s="6" t="n">
+        <v>0.000168</v>
+      </c>
       <c r="T20" s="6" t="inlineStr"/>
-      <c r="U20" s="7" t="inlineStr"/>
-      <c r="V20" s="6" t="inlineStr"/>
-      <c r="W20" s="6" t="inlineStr"/>
-      <c r="X20" s="6" t="inlineStr"/>
+      <c r="U20" s="7" t="inlineStr">
+        <is>
+          <t>GAGCTGGAACATGTTCTGGTTGCAGCCGGAGGATCCTTGCCGCGTTTACAATCTCTGTGGTCAATTAGGGTTTTGTAGCAGCGAATTGCTCAAGCCCTGTGC</t>
+        </is>
+      </c>
+      <c r="V20" s="6" t="n">
+        <v>101</v>
+      </c>
+      <c r="W20" s="6" t="n">
+        <v>51.9607843137255</v>
+      </c>
+      <c r="X20" s="6" t="n">
+        <v>-6.424409866333008</v>
+      </c>
       <c r="Y20" s="6" t="inlineStr"/>
-      <c r="Z20" s="6" t="inlineStr"/>
+      <c r="Z20" s="6" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>CP002687.1</t>
+        </is>
+      </c>
+      <c r="B21" s="7" t="inlineStr">
+        <is>
+          <t>GTATGCACGACTGGATCAC</t>
+        </is>
+      </c>
+      <c r="C21" s="6" t="n">
+        <v>58.01929187670885</v>
+      </c>
+      <c r="D21" s="6" t="n">
+        <v>1.585081350393057</v>
+      </c>
+      <c r="E21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G21" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H21" s="7" t="inlineStr">
+        <is>
+          <t>GTAGTTGTCGAACCTGGTC</t>
+        </is>
+      </c>
+      <c r="I21" s="6" t="n">
+        <v>57.48615986233125</v>
+      </c>
+      <c r="J21" s="6" t="n">
+        <v>1.07962961135296</v>
+      </c>
+      <c r="K21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="M21" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="N21" s="6" t="n">
+        <v>2.664710961746017</v>
+      </c>
+      <c r="O21" s="7" t="inlineStr">
+        <is>
+          <t>GCCGCCACACGCACGGAGGT</t>
+        </is>
+      </c>
+      <c r="P21" s="6" t="n">
+        <v>64.65986280657165</v>
+      </c>
+      <c r="Q21" s="6" t="n">
+        <v>0.3401371934283475</v>
+      </c>
+      <c r="R21" s="6" t="n">
+        <v>-1.617270469665527</v>
+      </c>
+      <c r="S21" s="6" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="T21" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="U21" s="7" t="inlineStr">
+        <is>
+          <t>GTATGCACGACTGGATCACTGAGAACCTCCGTGCGTGTGGCGGCACTTATCAGACATGTATCTGCGCCGTACCTTTCTTGGCAAAAAAGCAAGGTCTCGTGACCGTCACGTGCGATCCCAAGAACATCGAACACATGCTCAAGACCAGGTTCGACAACTACC</t>
+        </is>
+      </c>
+      <c r="V21" s="6" t="n">
+        <v>161</v>
+      </c>
+      <c r="W21" s="6" t="n">
+        <v>52.46913580246913</v>
+      </c>
+      <c r="X21" s="6" t="n">
+        <v>-10.59030723571777</v>
+      </c>
+      <c r="Y21" s="6" t="inlineStr"/>
+      <c r="Z21" s="6" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
fixed --snp in direct_mode
</commit_message>
<xml_diff>
--- a/ddprimer/test_data/Primers/Primers_fasta1.xlsx
+++ b/ddprimer/test_data/Primers/Primers_fasta1.xlsx
@@ -466,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z21"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -668,7 +668,7 @@
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
         <is>
-          <t>CP002684.1</t>
+          <t>PDH-E1 ALPHA</t>
         </is>
       </c>
       <c r="B3" s="7" t="inlineStr">
@@ -748,17 +748,21 @@
       <c r="X3" s="6" t="n">
         <v>-8.800433158874512</v>
       </c>
-      <c r="Y3" s="6" t="inlineStr"/>
+      <c r="Y3" s="6" t="inlineStr">
+        <is>
+          <t>CP002684.1</t>
+        </is>
+      </c>
       <c r="Z3" s="6" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>48586</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
         <is>
-          <t>CP002684.1</t>
+          <t>PDH-E1 ALPHA</t>
         </is>
       </c>
       <c r="B4" s="7" t="inlineStr">
@@ -838,229 +842,239 @@
       <c r="X4" s="6" t="n">
         <v>-8.800433158874512</v>
       </c>
-      <c r="Y4" s="6" t="inlineStr"/>
+      <c r="Y4" s="6" t="inlineStr">
+        <is>
+          <t>CP002684.1</t>
+        </is>
+      </c>
       <c r="Z4" s="6" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>48598</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
         <is>
-          <t>CP002684.1</t>
+          <t>CYP703A2</t>
         </is>
       </c>
       <c r="B5" s="7" t="inlineStr">
         <is>
-          <t>GAATCTAATCCGCCGAGTC</t>
+          <t>GAACGATCCCGATACCATC</t>
         </is>
       </c>
       <c r="C5" s="6" t="n">
-        <v>57.49691898952096</v>
+        <v>57.18013716608459</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>1.068870484163245</v>
+        <v>1.385652307599617</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>0</v>
+        <v>-0.8097348213195801</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>0.007</v>
       </c>
-      <c r="G5" s="6" t="n">
+      <c r="G5" s="6" t="inlineStr"/>
+      <c r="H5" s="7" t="inlineStr">
+        <is>
+          <t>CACATCCATACGCTAGGTG</t>
+        </is>
+      </c>
+      <c r="I5" s="6" t="n">
+        <v>57.40147050241876</v>
+      </c>
+      <c r="J5" s="6" t="n">
+        <v>1.164318971265448</v>
+      </c>
+      <c r="K5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="M5" s="6" t="n">
         <v>3.7</v>
       </c>
-      <c r="H5" s="7" t="inlineStr">
-        <is>
-          <t>CGCATAGAATCTGAGTCTCC</t>
-        </is>
-      </c>
-      <c r="I5" s="6" t="n">
-        <v>57.39128463697756</v>
-      </c>
-      <c r="J5" s="6" t="n">
-        <v>1.358715363022441</v>
-      </c>
-      <c r="K5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="M5" s="6" t="n">
-        <v>1.1</v>
-      </c>
       <c r="N5" s="6" t="n">
-        <v>2.427585847185686</v>
+        <v>2.549971278865065</v>
       </c>
       <c r="O5" s="7" t="inlineStr">
         <is>
-          <t>CCGACGCGCCGAGAAAACTCCCG</t>
+          <t>TCGAGACCCAAAACACTCGCCGCAGT</t>
         </is>
       </c>
       <c r="P5" s="6" t="n">
-        <v>64.42590694670616</v>
+        <v>64.30135325099201</v>
       </c>
       <c r="Q5" s="6" t="n">
-        <v>3.574093053293836</v>
+        <v>6.698646749007992</v>
       </c>
       <c r="R5" s="6" t="n">
-        <v>0</v>
+        <v>-1.419864654541016</v>
       </c>
       <c r="S5" s="6" t="n">
-        <v>4.81e-05</v>
+        <v>1.51e-06</v>
       </c>
       <c r="T5" s="6" t="n">
-        <v>1.1</v>
+        <v>1.4</v>
       </c>
       <c r="U5" s="7" t="inlineStr">
         <is>
-          <t>GAATCTAATCCGCCGAGTCAAACCTAAGACGATCGTCGAAGTCGGGAGTTTTCTCGGCGCGTCGGCGATACACATGGCGAATCTCACGCGCCGACTTGGGCTCGAGGAGACTCAGATTCTATGCGT</t>
+          <t>GAACGATCCCGATACCATCCGTGAGATTCTTTTGCGGCAGGACGATGTTTTTTCATCGAGACCCAAAACACTCGCCGCAGTCCACCTAGCGTATGGATGTGG</t>
         </is>
       </c>
       <c r="V5" s="6" t="n">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="W5" s="6" t="n">
-        <v>55.55555555555556</v>
+        <v>51.9607843137255</v>
       </c>
       <c r="X5" s="6" t="n">
-        <v>-12.9314661026001</v>
-      </c>
-      <c r="Y5" s="6" t="inlineStr"/>
+        <v>-5.947404861450195</v>
+      </c>
+      <c r="Y5" s="6" t="inlineStr">
+        <is>
+          <t>CP002684.1</t>
+        </is>
+      </c>
       <c r="Z5" s="6" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>112527</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
         <is>
-          <t>CP002684.1</t>
+          <t>CYP703A2</t>
         </is>
       </c>
       <c r="B6" s="7" t="inlineStr">
         <is>
-          <t>CCGAGTCAAACCTAAGACG</t>
+          <t>CAACGAACGATCCCGATAC</t>
         </is>
       </c>
       <c r="C6" s="6" t="n">
-        <v>57.57714328942353</v>
+        <v>58.1158368244387</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>1.142932763107741</v>
+        <v>1.681626298122911</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>0</v>
+        <v>-0.8097348213195801</v>
       </c>
       <c r="F6" s="6" t="n">
         <v>0.007</v>
       </c>
       <c r="G6" s="6" t="n">
-        <v>1.1</v>
+        <v>3.7</v>
       </c>
       <c r="H6" s="7" t="inlineStr">
         <is>
-          <t>AGAATCTGAGTCTCCTCGAG</t>
+          <t>ATCCATACGCTAGGTGGAC</t>
         </is>
       </c>
       <c r="I6" s="6" t="n">
-        <v>57.76917945968336</v>
+        <v>58.25082796726878</v>
       </c>
       <c r="J6" s="6" t="n">
-        <v>1.519179459683357</v>
+        <v>1.816617440952985</v>
       </c>
       <c r="K6" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L6" s="6" t="n">
-        <v>0.002</v>
+        <v>0.007</v>
       </c>
       <c r="M6" s="6" t="n">
         <v>1.1</v>
       </c>
       <c r="N6" s="6" t="n">
-        <v>2.662112222791098</v>
+        <v>3.498243739075896</v>
       </c>
       <c r="O6" s="7" t="inlineStr">
         <is>
-          <t>CCGACGCGCCGAGAAAACTCCCG</t>
+          <t>TCATCGAGACCCAAAACACTCGCCGCA</t>
         </is>
       </c>
       <c r="P6" s="6" t="n">
-        <v>64.42590694670616</v>
+        <v>64.20487603053124</v>
       </c>
       <c r="Q6" s="6" t="n">
-        <v>3.574093053293836</v>
+        <v>7.795123969468762</v>
       </c>
       <c r="R6" s="6" t="n">
-        <v>0</v>
+        <v>-1.419864654541016</v>
       </c>
       <c r="S6" s="6" t="n">
-        <v>4.81e-05</v>
+        <v>5.4e-07</v>
       </c>
       <c r="T6" s="6" t="n">
-        <v>1.1</v>
+        <v>0.042</v>
       </c>
       <c r="U6" s="7" t="inlineStr">
         <is>
-          <t>CCGAGTCAAACCTAAGACGATCGTCGAAGTCGGGAGTTTTCTCGGCGCGTCGGCGATACACATGGCGAATCTCACGCGCCGACTTGGGCTCGAGGAGACTCAGATTCTA</t>
+          <t>CAACGAACGATCCCGATACCATCCGTGAGATTCTTTTGCGGCAGGACGATGTTTTTTCATCGAGACCCAAAACACTCGCCGCAGTCCACCTAGCGTATGGATG</t>
         </is>
       </c>
       <c r="V6" s="6" t="n">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="W6" s="6" t="n">
-        <v>56.88073394495413</v>
+        <v>51.45631067961165</v>
       </c>
       <c r="X6" s="6" t="n">
-        <v>-12.9314661026001</v>
-      </c>
-      <c r="Y6" s="6" t="inlineStr"/>
+        <v>-5.947404861450195</v>
+      </c>
+      <c r="Y6" s="6" t="inlineStr">
+        <is>
+          <t>CP002684.1</t>
+        </is>
+      </c>
       <c r="Z6" s="6" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>112523</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
         <is>
-          <t>CP002684.1</t>
+          <t>At17.1</t>
         </is>
       </c>
       <c r="B7" s="7" t="inlineStr">
         <is>
-          <t>CTAATCCGCCGAGTCAAAC</t>
+          <t>GTCTTCCGATCTCTCCATAC</t>
         </is>
       </c>
       <c r="C7" s="6" t="n">
-        <v>58.31982523388075</v>
+        <v>56.72627428247569</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>1.885614707564958</v>
+        <v>2.023725717524314</v>
       </c>
       <c r="E7" s="6" t="n">
         <v>0</v>
       </c>
       <c r="F7" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="G7" s="6" t="n">
-        <v>3.7</v>
+        <v>0.3</v>
       </c>
       <c r="H7" s="7" t="inlineStr">
         <is>
-          <t>CGTCGACGCATAGAATCTG</t>
+          <t>CTCAGCTTTGGGAATCCTC</t>
         </is>
       </c>
       <c r="I7" s="6" t="n">
-        <v>58.20901248311378</v>
+        <v>57.50429449531657</v>
       </c>
       <c r="J7" s="6" t="n">
-        <v>1.77480195679799</v>
+        <v>1.07008396900078</v>
       </c>
       <c r="K7" s="6" t="n">
         <v>0</v>
@@ -1072,83 +1086,89 @@
         <v>1.1</v>
       </c>
       <c r="N7" s="6" t="n">
-        <v>3.660416664362948</v>
+        <v>3.093809686525095</v>
       </c>
       <c r="O7" s="7" t="inlineStr">
         <is>
-          <t>CCGACGCGCCGAGAAAACTCCCG</t>
+          <t>CCTCCGTCGTCCATCCTCCTGGTGGT</t>
         </is>
       </c>
       <c r="P7" s="6" t="n">
-        <v>64.42590694670616</v>
+        <v>64.72158538224431</v>
       </c>
       <c r="Q7" s="6" t="n">
-        <v>3.574093053293836</v>
+        <v>6.278414617755686</v>
       </c>
       <c r="R7" s="6" t="n">
         <v>0</v>
       </c>
       <c r="S7" s="6" t="n">
-        <v>4.81e-05</v>
+        <v>1.51e-06</v>
       </c>
       <c r="T7" s="6" t="n">
-        <v>1.1</v>
+        <v>0.4</v>
       </c>
       <c r="U7" s="7" t="inlineStr">
         <is>
-          <t>CTAATCCGCCGAGTCAAACCTAAGACGATCGTCGAAGTCGGGAGTTTTCTCGGCGCGTCGGCGATACACATGGCGAATCTCACGCGCCGACTTGGGCTCGAGGAGACTCAGATTCTATGCGTCGACGA</t>
+          <t>GTCTTCCGATCTCTCCATACTCAAACCACCAGGAGGATGGACGACGGAGGAAGAAGAAGGAGCGGTGAGGAGGGTGAAGGTGAGGATTCCCAAAGCTGAGC</t>
         </is>
       </c>
       <c r="V7" s="6" t="n">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="W7" s="6" t="n">
-        <v>57.03125</v>
+        <v>55.44554455445545</v>
       </c>
       <c r="X7" s="6" t="n">
-        <v>-13.85025310516357</v>
-      </c>
-      <c r="Y7" s="6" t="inlineStr"/>
+        <v>-4.261404037475586</v>
+      </c>
+      <c r="Y7" s="6" t="inlineStr">
+        <is>
+          <t>CP002685.1</t>
+        </is>
+      </c>
       <c r="Z7" s="6" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>164431</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>CP002684.1</t>
+          <t>At17.1</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>GAACGATCCCGATACCATC</t>
+          <t>CATACTCAAACCACCAGGAG</t>
         </is>
       </c>
       <c r="C8" s="6" t="n">
-        <v>57.18013716608459</v>
+        <v>57.70701631138252</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>1.385652307599617</v>
+        <v>1.457016311382517</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>-0.8097348213195801</v>
+        <v>-0.7797346115112305</v>
       </c>
       <c r="F8" s="6" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="G8" s="6" t="inlineStr"/>
+        <v>0.002</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>1.1</v>
+      </c>
       <c r="H8" s="7" t="inlineStr">
         <is>
-          <t>CACATCCATACGCTAGGTG</t>
+          <t>GGTGGCTCCTTCTTTAACG</t>
         </is>
       </c>
       <c r="I8" s="6" t="n">
-        <v>57.40147050241876</v>
+        <v>58.14276553363504</v>
       </c>
       <c r="J8" s="6" t="n">
-        <v>1.164318971265448</v>
+        <v>1.708555007319251</v>
       </c>
       <c r="K8" s="6" t="n">
         <v>0</v>
@@ -1160,175 +1180,183 @@
         <v>3.7</v>
       </c>
       <c r="N8" s="6" t="n">
-        <v>2.549971278865065</v>
+        <v>3.165571318701769</v>
       </c>
       <c r="O8" s="7" t="inlineStr">
         <is>
-          <t>TCGAGACCCAAAACACTCGCCGCAGT</t>
+          <t>TCCTCACCTTCACCCTCCTCACCGCT</t>
         </is>
       </c>
       <c r="P8" s="6" t="n">
-        <v>64.30135325099201</v>
+        <v>64.17251465903956</v>
       </c>
       <c r="Q8" s="6" t="n">
-        <v>6.698646749007992</v>
+        <v>6.827485340960436</v>
       </c>
       <c r="R8" s="6" t="n">
-        <v>-1.419864654541016</v>
+        <v>0</v>
       </c>
       <c r="S8" s="6" t="n">
         <v>1.51e-06</v>
       </c>
       <c r="T8" s="6" t="n">
-        <v>1.4</v>
+        <v>0.033</v>
       </c>
       <c r="U8" s="7" t="inlineStr">
         <is>
-          <t>GAACGATCCCGATACCATCCGTGAGATTCTTTTGCGGCAGGACGATGTTTTTTCATCGAGACCCAAAACACTCGCCGCAGTCCACCTAGCGTATGGATGTGG</t>
+          <t>CATACTCAAACCACCAGGAGGATGGACGACGGAGGAAGAAGAAGGAGCGGTGAGGAGGGTGAAGGTGAGGATTCCCAAAGCTGAGCTTGAAAAGCTCGTTAAAGAAGGAGCCACCG</t>
         </is>
       </c>
       <c r="V8" s="6" t="n">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="W8" s="6" t="n">
-        <v>51.9607843137255</v>
+        <v>53.44827586206896</v>
       </c>
       <c r="X8" s="6" t="n">
-        <v>-5.947404861450195</v>
-      </c>
-      <c r="Y8" s="6" t="inlineStr"/>
+        <v>-5.429211139678955</v>
+      </c>
+      <c r="Y8" s="6" t="inlineStr">
+        <is>
+          <t>CP002685.1</t>
+        </is>
+      </c>
       <c r="Z8" s="6" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>164446</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>CP002684.1</t>
+          <t>MTO1</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>CAACGAACGATCCCGATAC</t>
+          <t>CTGGTGGATCTAGGAGGTAC</t>
         </is>
       </c>
       <c r="C9" s="6" t="n">
-        <v>58.1158368244387</v>
+        <v>58.11536079407438</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v>1.681626298122911</v>
+        <v>1.865360794074377</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>-0.8097348213195801</v>
+        <v>0</v>
       </c>
       <c r="F9" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="G9" s="6" t="n">
-        <v>3.7</v>
+        <v>0.3</v>
       </c>
       <c r="H9" s="7" t="inlineStr">
         <is>
-          <t>ATCCATACGCTAGGTGGAC</t>
+          <t>GGGATCAGGGAGAAGATAGG</t>
         </is>
       </c>
       <c r="I9" s="6" t="n">
-        <v>58.25082796726878</v>
+        <v>58.1693460818891</v>
       </c>
       <c r="J9" s="6" t="n">
-        <v>1.816617440952985</v>
+        <v>1.919346081889103</v>
       </c>
       <c r="K9" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L9" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="M9" s="6" t="n">
         <v>1.1</v>
       </c>
       <c r="N9" s="6" t="n">
-        <v>3.498243739075896</v>
+        <v>3.784706875963479</v>
       </c>
       <c r="O9" s="7" t="inlineStr">
         <is>
-          <t>TCATCGAGACCCAAAACACTCGCCGCA</t>
+          <t>CCGATGGGAGCCTCACTGTTCATGCCG</t>
         </is>
       </c>
       <c r="P9" s="6" t="n">
-        <v>64.20487603053124</v>
+        <v>64.81452393084095</v>
       </c>
       <c r="Q9" s="6" t="n">
-        <v>7.795123969468762</v>
+        <v>7.185476069159051</v>
       </c>
       <c r="R9" s="6" t="n">
-        <v>-1.419864654541016</v>
+        <v>0</v>
       </c>
       <c r="S9" s="6" t="n">
         <v>5.4e-07</v>
       </c>
       <c r="T9" s="6" t="n">
-        <v>0.042</v>
+        <v>0.51</v>
       </c>
       <c r="U9" s="7" t="inlineStr">
         <is>
-          <t>CAACGAACGATCCCGATACCATCCGTGAGATTCTTTTGCGGCAGGACGATGTTTTTTCATCGAGACCCAAAACACTCGCCGCAGTCCACCTAGCGTATGGATG</t>
+          <t>CTGGTGGATCTAGGAGGTACCGGCATGAACAGTGAGGCTCCCATCGGAGCTCAAGAAAGAATGTTTGGAATCCGTCAGCTGTACACTACCTATCTTCTCCCTGATCCCC</t>
         </is>
       </c>
       <c r="V9" s="6" t="n">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="W9" s="6" t="n">
-        <v>51.45631067961165</v>
+        <v>52.29357798165137</v>
       </c>
       <c r="X9" s="6" t="n">
-        <v>-5.947404861450195</v>
-      </c>
-      <c r="Y9" s="6" t="inlineStr"/>
+        <v>-3.461651563644409</v>
+      </c>
+      <c r="Y9" s="6" t="inlineStr">
+        <is>
+          <t>CP002686.1</t>
+        </is>
+      </c>
       <c r="Z9" s="6" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>41300</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>CP002685.1</t>
+          <t>MTO1</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>TCCGTCGACAGAGTCAATC</t>
+          <t>CTGAATCTGGTGGATCTAGG</t>
         </is>
       </c>
       <c r="C10" s="6" t="n">
-        <v>58.81843131961955</v>
+        <v>56.59552606387956</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>2.384220793303758</v>
+        <v>2.154473936120439</v>
       </c>
       <c r="E10" s="6" t="n">
         <v>0</v>
       </c>
       <c r="F10" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="G10" s="6" t="n">
-        <v>3.7</v>
+        <v>1.1</v>
       </c>
       <c r="H10" s="7" t="inlineStr">
         <is>
-          <t>TCATGACTCGGATCTTAGCC</t>
+          <t>CAGGGAGAAGATAGGTAGTG</t>
         </is>
       </c>
       <c r="I10" s="6" t="n">
-        <v>58.78643594651186</v>
+        <v>55.9357109944566</v>
       </c>
       <c r="J10" s="6" t="n">
-        <v>2.536435946511858</v>
+        <v>2.814289005543401</v>
       </c>
       <c r="K10" s="6" t="n">
         <v>0</v>
@@ -1340,85 +1368,89 @@
         <v>3.7</v>
       </c>
       <c r="N10" s="6" t="n">
-        <v>4.920656739815616</v>
+        <v>4.96876294166384</v>
       </c>
       <c r="O10" s="7" t="inlineStr">
         <is>
-          <t>TGCAAGCCCACGCCGCCGAT</t>
+          <t>CCGATGGGAGCCTCACTGTTCATGCCG</t>
         </is>
       </c>
       <c r="P10" s="6" t="n">
-        <v>64.4500508334425</v>
+        <v>64.81452393084095</v>
       </c>
       <c r="Q10" s="6" t="n">
-        <v>0.5499491665574965</v>
+        <v>7.185476069159051</v>
       </c>
       <c r="R10" s="6" t="n">
-        <v>-0.7097349166870117</v>
+        <v>0</v>
       </c>
       <c r="S10" s="6" t="n">
-        <v>0.002</v>
+        <v>5.4e-07</v>
       </c>
       <c r="T10" s="6" t="n">
-        <v>0.3</v>
+        <v>0.51</v>
       </c>
       <c r="U10" s="7" t="inlineStr">
         <is>
-          <t>TCCGTCGACAGAGTCAATCTTATGCAAGCCCACGCCGCCGATCTCGTCAGAGATGCTTCCTTGAACGACCGAGTGGAGCTCACAGTCCGCGGAGACGTGGGGGCTAAGATCCGAGTCATGAA</t>
+          <t>CTGAATCTGGTGGATCTAGGAGGTACCGGCATGAACAGTGAGGCTCCCATCGGAGCTCAAGAAAGAATGTTTGGAATCCGTCAGCTGTACACTACCTATCTTCTCCCTGA</t>
         </is>
       </c>
       <c r="V10" s="6" t="n">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="W10" s="6" t="n">
-        <v>57.37704918032787</v>
+        <v>50</v>
       </c>
       <c r="X10" s="6" t="n">
-        <v>-5.358549118041992</v>
-      </c>
-      <c r="Y10" s="6" t="inlineStr"/>
+        <v>-3.461651563644409</v>
+      </c>
+      <c r="Y10" s="6" t="inlineStr">
+        <is>
+          <t>CP002686.1</t>
+        </is>
+      </c>
       <c r="Z10" s="6" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>41294</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>CP002685.1</t>
+          <t>XSP1</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
         <is>
-          <t>GTCTTCCGATCTCTCCATAC</t>
+          <t>CTACGACATGGACGACATC</t>
         </is>
       </c>
       <c r="C11" s="6" t="n">
-        <v>56.72627428247569</v>
+        <v>57.44369071181501</v>
       </c>
       <c r="D11" s="6" t="n">
-        <v>2.023725717524314</v>
+        <v>1.1220987618692</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>0</v>
+        <v>-0.3097348213195801</v>
       </c>
       <c r="F11" s="6" t="n">
-        <v>0.002</v>
+        <v>0.007</v>
       </c>
       <c r="G11" s="6" t="n">
-        <v>0.3</v>
+        <v>1.1</v>
       </c>
       <c r="H11" s="7" t="inlineStr">
         <is>
-          <t>CTCAGCTTTGGGAATCCTC</t>
+          <t>GACAATGGAGGAACAGCTC</t>
         </is>
       </c>
       <c r="I11" s="6" t="n">
-        <v>57.50429449531657</v>
+        <v>57.83082272420569</v>
       </c>
       <c r="J11" s="6" t="n">
-        <v>1.07008396900078</v>
+        <v>1.396612197889898</v>
       </c>
       <c r="K11" s="6" t="n">
         <v>0</v>
@@ -1430,85 +1462,89 @@
         <v>1.1</v>
       </c>
       <c r="N11" s="6" t="n">
-        <v>3.093809686525095</v>
+        <v>2.518710959759098</v>
       </c>
       <c r="O11" s="7" t="inlineStr">
         <is>
-          <t>CCTCCGTCGTCCATCCTCCTGGTGGT</t>
+          <t>AGCTCCATTGGTGGGTACACGCTCCG</t>
         </is>
       </c>
       <c r="P11" s="6" t="n">
-        <v>64.72158538224431</v>
+        <v>64.22598535419934</v>
       </c>
       <c r="Q11" s="6" t="n">
-        <v>6.278414617755686</v>
+        <v>6.774014645800662</v>
       </c>
       <c r="R11" s="6" t="n">
-        <v>0</v>
+        <v>-0.7341697216033936</v>
       </c>
       <c r="S11" s="6" t="n">
         <v>1.51e-06</v>
       </c>
       <c r="T11" s="6" t="n">
-        <v>0.4</v>
+        <v>1.4</v>
       </c>
       <c r="U11" s="7" t="inlineStr">
         <is>
-          <t>GTCTTCCGATCTCTCCATACTCAAACCACCAGGAGGATGGACGACGGAGGAAGAAGAAGGAGCGGTGAGGAGGGTGAAGGTGAGGATTCCCAAAGCTGAGC</t>
+          <t>CTACGACATGGACGACATCTCCTATGTTCAGTTCTTGTGCGGCGAAGGCTACAACGCAACCACTCTAGCTCCATTGGTGGGTACACGCTCCGTGAGCTGTTCCTCCATTGTCC</t>
         </is>
       </c>
       <c r="V11" s="6" t="n">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="W11" s="6" t="n">
-        <v>55.44554455445545</v>
+        <v>53.98230088495575</v>
       </c>
       <c r="X11" s="6" t="n">
-        <v>-4.261404037475586</v>
-      </c>
-      <c r="Y11" s="6" t="inlineStr"/>
+        <v>-6.521465301513672</v>
+      </c>
+      <c r="Y11" s="6" t="inlineStr">
+        <is>
+          <t>CP002687.1</t>
+        </is>
+      </c>
       <c r="Z11" s="6" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>96840</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>CP002685.1</t>
+          <t>XSP1</t>
         </is>
       </c>
       <c r="B12" s="7" t="inlineStr">
         <is>
-          <t>CATACTCAAACCACCAGGAG</t>
+          <t>CTGGCTTAGTCTACGACATG</t>
         </is>
       </c>
       <c r="C12" s="6" t="n">
-        <v>57.70701631138252</v>
+        <v>57.6139686963578</v>
       </c>
       <c r="D12" s="6" t="n">
-        <v>1.457016311382517</v>
+        <v>1.363968696357801</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>-0.7797346115112305</v>
+        <v>0</v>
       </c>
       <c r="F12" s="6" t="n">
         <v>0.002</v>
       </c>
       <c r="G12" s="6" t="n">
-        <v>1.1</v>
+        <v>3.7</v>
       </c>
       <c r="H12" s="7" t="inlineStr">
         <is>
-          <t>GGTGGCTCCTTCTTTAACG</t>
+          <t>AGGGACAATGGAGGAACAG</t>
         </is>
       </c>
       <c r="I12" s="6" t="n">
-        <v>58.14276553363504</v>
+        <v>58.60725372965351</v>
       </c>
       <c r="J12" s="6" t="n">
-        <v>1.708555007319251</v>
+        <v>2.173043203337716</v>
       </c>
       <c r="K12" s="6" t="n">
         <v>0</v>
@@ -1517,88 +1553,92 @@
         <v>0.007</v>
       </c>
       <c r="M12" s="6" t="n">
-        <v>3.7</v>
+        <v>1.1</v>
       </c>
       <c r="N12" s="6" t="n">
-        <v>3.165571318701769</v>
+        <v>3.537011899695518</v>
       </c>
       <c r="O12" s="7" t="inlineStr">
         <is>
-          <t>TCCTCACCTTCACCCTCCTCACCGCT</t>
+          <t>AGCTCCATTGGTGGGTACACGCTCCG</t>
         </is>
       </c>
       <c r="P12" s="6" t="n">
-        <v>64.17251465903956</v>
+        <v>64.22598535419934</v>
       </c>
       <c r="Q12" s="6" t="n">
-        <v>6.827485340960436</v>
+        <v>6.774014645800662</v>
       </c>
       <c r="R12" s="6" t="n">
-        <v>0</v>
+        <v>-0.7341697216033936</v>
       </c>
       <c r="S12" s="6" t="n">
         <v>1.51e-06</v>
       </c>
       <c r="T12" s="6" t="n">
-        <v>0.033</v>
+        <v>1.4</v>
       </c>
       <c r="U12" s="7" t="inlineStr">
         <is>
-          <t>CATACTCAAACCACCAGGAGGATGGACGACGGAGGAAGAAGAAGGAGCGGTGAGGAGGGTGAAGGTGAGGATTCCCAAAGCTGAGCTTGAAAAGCTCGTTAAAGAAGGAGCCACCG</t>
+          <t>CTGGCTTAGTCTACGACATGGACGACATCTCCTATGTTCAGTTCTTGTGCGGCGAAGGCTACAACGCAACCACTCTAGCTCCATTGGTGGGTACACGCTCCGTGAGCTGTTCCTCCATTGTCCCTG</t>
         </is>
       </c>
       <c r="V12" s="6" t="n">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="W12" s="6" t="n">
-        <v>53.44827586206896</v>
+        <v>53.96825396825397</v>
       </c>
       <c r="X12" s="6" t="n">
-        <v>-5.429211139678955</v>
-      </c>
-      <c r="Y12" s="6" t="inlineStr"/>
+        <v>-6.521465301513672</v>
+      </c>
+      <c r="Y12" s="6" t="inlineStr">
+        <is>
+          <t>CP002687.1</t>
+        </is>
+      </c>
       <c r="Z12" s="6" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>96830</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="inlineStr">
         <is>
-          <t>CP002686.1</t>
+          <t>XSP1</t>
         </is>
       </c>
       <c r="B13" s="7" t="inlineStr">
         <is>
-          <t>CTGGTGGATCTAGGAGGTAC</t>
+          <t>CCCAACAATCCAACTCACG</t>
         </is>
       </c>
       <c r="C13" s="6" t="n">
-        <v>58.11536079407438</v>
+        <v>58.74250943646473</v>
       </c>
       <c r="D13" s="6" t="n">
-        <v>1.865360794074377</v>
+        <v>2.308298910148938</v>
       </c>
       <c r="E13" s="6" t="n">
         <v>0</v>
       </c>
       <c r="F13" s="6" t="n">
-        <v>0.002</v>
+        <v>0.007</v>
       </c>
       <c r="G13" s="6" t="n">
-        <v>0.3</v>
+        <v>3.7</v>
       </c>
       <c r="H13" s="7" t="inlineStr">
         <is>
-          <t>GGGATCAGGGAGAAGATAGG</t>
+          <t>CCACCACTTTGAAGCTTCTC</t>
         </is>
       </c>
       <c r="I13" s="6" t="n">
-        <v>58.1693460818891</v>
+        <v>58.87532172899461</v>
       </c>
       <c r="J13" s="6" t="n">
-        <v>1.919346081889103</v>
+        <v>2.625321728994606</v>
       </c>
       <c r="K13" s="6" t="n">
         <v>0</v>
@@ -1607,158 +1647,164 @@
         <v>0.002</v>
       </c>
       <c r="M13" s="6" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="N13" s="6" t="n">
+        <v>4.933620639143545</v>
+      </c>
+      <c r="O13" s="7" t="inlineStr">
+        <is>
+          <t>CCGCCACCGTCCGAGCACCG</t>
+        </is>
+      </c>
+      <c r="P13" s="6" t="n">
+        <v>64.7335341111355</v>
+      </c>
+      <c r="Q13" s="6" t="n">
+        <v>0.2664658888645022</v>
+      </c>
+      <c r="R13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" s="6" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="T13" s="6" t="n">
         <v>1.1</v>
       </c>
-      <c r="N13" s="6" t="n">
-        <v>3.784706875963479</v>
-      </c>
-      <c r="O13" s="7" t="inlineStr">
-        <is>
-          <t>CCGATGGGAGCCTCACTGTTCATGCCG</t>
-        </is>
-      </c>
-      <c r="P13" s="6" t="n">
-        <v>64.81452393084095</v>
-      </c>
-      <c r="Q13" s="6" t="n">
-        <v>7.185476069159051</v>
-      </c>
-      <c r="R13" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S13" s="6" t="n">
-        <v>5.4e-07</v>
-      </c>
-      <c r="T13" s="6" t="n">
-        <v>0.51</v>
-      </c>
       <c r="U13" s="7" t="inlineStr">
         <is>
-          <t>CTGGTGGATCTAGGAGGTACCGGCATGAACAGTGAGGCTCCCATCGGAGCTCAAGAAAGAATGTTTGGAATCCGTCAGCTGTACACTACCTATCTTCTCCCTGATCCCC</t>
+          <t>CCCAACAATCCAACTCACGTTGAGATCCGCCAAAACGTCCACATTGGCTGTGTTCAGGCGGAGAGTCACCAACGTGGGACCACCGTCGTCGGTCTACACCGCCACCGTCCGAGCACCGAAAGGAGTAGAAATCACGGTGGAGCCACAGAGTTTGTCATTTTCAAAGGCTTCACAAAAGAGAAGCTTCAAAGTGGTGGT</t>
         </is>
       </c>
       <c r="V13" s="6" t="n">
-        <v>108</v>
+        <v>197</v>
       </c>
       <c r="W13" s="6" t="n">
-        <v>52.29357798165137</v>
+        <v>53.03030303030303</v>
       </c>
       <c r="X13" s="6" t="n">
-        <v>-3.461651563644409</v>
-      </c>
-      <c r="Y13" s="6" t="inlineStr"/>
+        <v>-17.26604652404785</v>
+      </c>
+      <c r="Y13" s="6" t="inlineStr">
+        <is>
+          <t>CP002687.1</t>
+        </is>
+      </c>
       <c r="Z13" s="6" t="inlineStr">
         <is>
-          <t>72</t>
+          <t>96981</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
         <is>
-          <t>CP002686.1</t>
+          <t>RLK4</t>
         </is>
       </c>
       <c r="B14" s="7" t="inlineStr">
         <is>
-          <t>CTGAATCTGGTGGATCTAGG</t>
+          <t>GAGCTGGAACATGTTCTGG</t>
         </is>
       </c>
       <c r="C14" s="6" t="n">
-        <v>56.59552606387956</v>
+        <v>58.13313451624401</v>
       </c>
       <c r="D14" s="6" t="n">
-        <v>2.154473936120439</v>
+        <v>1.698923989928222</v>
       </c>
       <c r="E14" s="6" t="n">
         <v>0</v>
       </c>
       <c r="F14" s="6" t="n">
-        <v>0.002</v>
+        <v>0.007</v>
       </c>
       <c r="G14" s="6" t="n">
         <v>1.1</v>
       </c>
       <c r="H14" s="7" t="inlineStr">
         <is>
-          <t>CAGGGAGAAGATAGGTAGTG</t>
+          <t>CACAGGGCTTGAGCAATTC</t>
         </is>
       </c>
       <c r="I14" s="6" t="n">
-        <v>55.9357109944566</v>
+        <v>59.11187222956136</v>
       </c>
       <c r="J14" s="6" t="n">
-        <v>2.814289005543401</v>
+        <v>2.677661703245565</v>
       </c>
       <c r="K14" s="6" t="n">
-        <v>0</v>
+        <v>-0.790266752243042</v>
       </c>
       <c r="L14" s="6" t="n">
-        <v>0.002</v>
+        <v>0.007</v>
       </c>
       <c r="M14" s="6" t="n">
         <v>3.7</v>
       </c>
       <c r="N14" s="6" t="n">
-        <v>4.96876294166384</v>
+        <v>4.376585693173787</v>
       </c>
       <c r="O14" s="7" t="inlineStr">
         <is>
-          <t>CCGATGGGAGCCTCACTGTTCATGCCG</t>
+          <t>ACGCGGCAAGGATCCTCCGGCT</t>
         </is>
       </c>
       <c r="P14" s="6" t="n">
-        <v>64.81452393084095</v>
+        <v>64.70494890469467</v>
       </c>
       <c r="Q14" s="6" t="n">
-        <v>7.185476069159051</v>
+        <v>2.295051095305325</v>
       </c>
       <c r="R14" s="6" t="n">
-        <v>0</v>
+        <v>-0.9579751491546631</v>
       </c>
       <c r="S14" s="6" t="n">
-        <v>5.4e-07</v>
-      </c>
-      <c r="T14" s="6" t="n">
-        <v>0.51</v>
-      </c>
+        <v>0.000168</v>
+      </c>
+      <c r="T14" s="6" t="inlineStr"/>
       <c r="U14" s="7" t="inlineStr">
         <is>
-          <t>CTGAATCTGGTGGATCTAGGAGGTACCGGCATGAACAGTGAGGCTCCCATCGGAGCTCAAGAAAGAATGTTTGGAATCCGTCAGCTGTACACTACCTATCTTCTCCCTGA</t>
+          <t>GAGCTGGAACATGTTCTGGTTGCAGCCGGAGGATCCTTGCCGCGTTTACAATCTCTGTGGTCAATTAGGGTTTTGTAGCAGCGAATTGCTCAAGCCCTGTGC</t>
         </is>
       </c>
       <c r="V14" s="6" t="n">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="W14" s="6" t="n">
-        <v>50</v>
+        <v>51.9607843137255</v>
       </c>
       <c r="X14" s="6" t="n">
-        <v>-3.461651563644409</v>
-      </c>
-      <c r="Y14" s="6" t="inlineStr"/>
+        <v>-6.424409866333008</v>
+      </c>
+      <c r="Y14" s="6" t="inlineStr">
+        <is>
+          <t>CP002687.1</t>
+        </is>
+      </c>
       <c r="Z14" s="6" t="inlineStr">
         <is>
-          <t>66</t>
+          <t>149753</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="6" t="inlineStr">
         <is>
-          <t>CP002686.1</t>
+          <t>CYP86A2</t>
         </is>
       </c>
       <c r="B15" s="7" t="inlineStr">
         <is>
-          <t>CTTGAGACTGAGGAATGCG</t>
+          <t>GTATGCACGACTGGATCAC</t>
         </is>
       </c>
       <c r="C15" s="6" t="n">
-        <v>57.93566240021704</v>
+        <v>58.01929187670885</v>
       </c>
       <c r="D15" s="6" t="n">
-        <v>1.501451873901249</v>
+        <v>1.585081350393057</v>
       </c>
       <c r="E15" s="6" t="n">
         <v>0</v>
@@ -1771,603 +1817,69 @@
       </c>
       <c r="H15" s="7" t="inlineStr">
         <is>
-          <t>CCTTACAGAACAACCACACC</t>
+          <t>GTAGTTGTCGAACCTGGTC</t>
         </is>
       </c>
       <c r="I15" s="6" t="n">
-        <v>58.51220659203409</v>
+        <v>57.48615986233125</v>
       </c>
       <c r="J15" s="6" t="n">
-        <v>2.26220659203409</v>
+        <v>1.07962961135296</v>
       </c>
       <c r="K15" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L15" s="6" t="n">
-        <v>0.002</v>
+        <v>0.007</v>
       </c>
       <c r="M15" s="6" t="n">
         <v>1.1</v>
       </c>
       <c r="N15" s="6" t="n">
-        <v>3.76365846593534</v>
+        <v>2.664710961746017</v>
       </c>
       <c r="O15" s="7" t="inlineStr">
         <is>
-          <t>GCTCTGAAAACAAGCACGGCTCGCCCA</t>
+          <t>GCCGCCACACGCACGGAGGT</t>
         </is>
       </c>
       <c r="P15" s="6" t="n">
-        <v>65.50373796818639</v>
+        <v>64.65986280657165</v>
       </c>
       <c r="Q15" s="6" t="n">
-        <v>7.503737968186385</v>
+        <v>0.3401371934283475</v>
       </c>
       <c r="R15" s="6" t="n">
-        <v>0</v>
+        <v>-1.617270469665527</v>
       </c>
       <c r="S15" s="6" t="n">
-        <v>5.4e-07</v>
+        <v>0.002</v>
       </c>
       <c r="T15" s="6" t="n">
-        <v>0.001</v>
+        <v>1.1</v>
       </c>
       <c r="U15" s="7" t="inlineStr">
         <is>
-          <t>CTTGAGACTGAGGAATGCGTCAAGAGCTCCAGCAACAAGAGGGGAATGTTTGAGTTGCCTCGTGTTCATCACCGTGAATTGGAAGCTGAGCTGAAGAAGATGGCTCCGCCTAATGGGCGAGCCGTGCTTGTTTTCAGAGCGAGGTGTGGTTGTTCTGTAAGGA</t>
+          <t>GTATGCACGACTGGATCACTGAGAACCTCCGTGCGTGTGGCGGCACTTATCAGACATGTATCTGCGCCGTACCTTTCTTGGCAAAAAAGCAAGGTCTCGTGACCGTCACGTGCGATCCCAAGAACATCGAACACATGCTCAAGACCAGGTTCGACAACTACC</t>
         </is>
       </c>
       <c r="V15" s="6" t="n">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="W15" s="6" t="n">
-        <v>51.53374233128834</v>
+        <v>52.46913580246913</v>
       </c>
       <c r="X15" s="6" t="n">
-        <v>-7.891154766082764</v>
-      </c>
-      <c r="Y15" s="6" t="inlineStr"/>
+        <v>-10.59030723571777</v>
+      </c>
+      <c r="Y15" s="6" t="inlineStr">
+        <is>
+          <t>CP002687.1</t>
+        </is>
+      </c>
       <c r="Z15" s="6" t="inlineStr">
         <is>
-          <t>31</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="6" t="inlineStr">
-        <is>
-          <t>CP002687.1</t>
-        </is>
-      </c>
-      <c r="B16" s="7" t="inlineStr">
-        <is>
-          <t>CCTAGAGTACACCGGTTCTC</t>
-        </is>
-      </c>
-      <c r="C16" s="6" t="n">
-        <v>58.72687468691566</v>
-      </c>
-      <c r="D16" s="6" t="n">
-        <v>2.476874686915664</v>
-      </c>
-      <c r="E16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="6" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="G16" s="6" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="H16" s="7" t="inlineStr">
-        <is>
-          <t>GAGACTCATTGGTTCGTGTC</t>
-        </is>
-      </c>
-      <c r="I16" s="6" t="n">
-        <v>58.3997252290801</v>
-      </c>
-      <c r="J16" s="6" t="n">
-        <v>2.149725229080104</v>
-      </c>
-      <c r="K16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" s="6" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="M16" s="6" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="N16" s="6" t="n">
-        <v>4.626599915995769</v>
-      </c>
-      <c r="O16" s="7" t="inlineStr">
-        <is>
-          <t>CGCGCCAGAATCAAGCCTCCTTCACG</t>
-        </is>
-      </c>
-      <c r="P16" s="6" t="n">
-        <v>64.0105612867751</v>
-      </c>
-      <c r="Q16" s="6" t="n">
-        <v>6.989438713224899</v>
-      </c>
-      <c r="R16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S16" s="6" t="n">
-        <v>1.51e-06</v>
-      </c>
-      <c r="T16" s="6" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="U16" s="7" t="inlineStr">
-        <is>
-          <t>CCTAGAGTACACCGGTTCTCCACAACTTGGGTGGAATCTTGAGCGTGAAGGAGGCTTGATTCTGGCGCGAGACACGAACCAATGAGTCTCA</t>
-        </is>
-      </c>
-      <c r="V16" s="6" t="n">
-        <v>90</v>
-      </c>
-      <c r="W16" s="6" t="n">
-        <v>52.74725274725275</v>
-      </c>
-      <c r="X16" s="6" t="n">
-        <v>-4.578721046447754</v>
-      </c>
-      <c r="Y16" s="6" t="inlineStr"/>
-      <c r="Z16" s="6" t="inlineStr">
-        <is>
-          <t>57</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="6" t="inlineStr">
-        <is>
-          <t>CP002687.1</t>
-        </is>
-      </c>
-      <c r="B17" s="7" t="inlineStr">
-        <is>
-          <t>CTACGACATGGACGACATC</t>
-        </is>
-      </c>
-      <c r="C17" s="6" t="n">
-        <v>57.44369071181501</v>
-      </c>
-      <c r="D17" s="6" t="n">
-        <v>1.1220987618692</v>
-      </c>
-      <c r="E17" s="6" t="n">
-        <v>-0.3097348213195801</v>
-      </c>
-      <c r="F17" s="6" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="G17" s="6" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="H17" s="7" t="inlineStr">
-        <is>
-          <t>GACAATGGAGGAACAGCTC</t>
-        </is>
-      </c>
-      <c r="I17" s="6" t="n">
-        <v>57.83082272420569</v>
-      </c>
-      <c r="J17" s="6" t="n">
-        <v>1.396612197889898</v>
-      </c>
-      <c r="K17" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" s="6" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="M17" s="6" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="N17" s="6" t="n">
-        <v>2.518710959759098</v>
-      </c>
-      <c r="O17" s="7" t="inlineStr">
-        <is>
-          <t>AGCTCCATTGGTGGGTACACGCTCCG</t>
-        </is>
-      </c>
-      <c r="P17" s="6" t="n">
-        <v>64.22598535419934</v>
-      </c>
-      <c r="Q17" s="6" t="n">
-        <v>6.774014645800662</v>
-      </c>
-      <c r="R17" s="6" t="n">
-        <v>-0.7341697216033936</v>
-      </c>
-      <c r="S17" s="6" t="n">
-        <v>1.51e-06</v>
-      </c>
-      <c r="T17" s="6" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="U17" s="7" t="inlineStr">
-        <is>
-          <t>CTACGACATGGACGACATCTCCTATGTTCAGTTCTTGTGCGGCGAAGGCTACAACGCAACCACTCTAGCTCCATTGGTGGGTACACGCTCCGTGAGCTGTTCCTCCATTGTCC</t>
-        </is>
-      </c>
-      <c r="V17" s="6" t="n">
-        <v>112</v>
-      </c>
-      <c r="W17" s="6" t="n">
-        <v>53.98230088495575</v>
-      </c>
-      <c r="X17" s="6" t="n">
-        <v>-6.521465301513672</v>
-      </c>
-      <c r="Y17" s="6" t="inlineStr"/>
-      <c r="Z17" s="6" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="6" t="inlineStr">
-        <is>
-          <t>CP002687.1</t>
-        </is>
-      </c>
-      <c r="B18" s="7" t="inlineStr">
-        <is>
-          <t>CTGGCTTAGTCTACGACATG</t>
-        </is>
-      </c>
-      <c r="C18" s="6" t="n">
-        <v>57.6139686963578</v>
-      </c>
-      <c r="D18" s="6" t="n">
-        <v>1.363968696357801</v>
-      </c>
-      <c r="E18" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" s="6" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="G18" s="6" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="H18" s="7" t="inlineStr">
-        <is>
-          <t>AGGGACAATGGAGGAACAG</t>
-        </is>
-      </c>
-      <c r="I18" s="6" t="n">
-        <v>58.60725372965351</v>
-      </c>
-      <c r="J18" s="6" t="n">
-        <v>2.173043203337716</v>
-      </c>
-      <c r="K18" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" s="6" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="M18" s="6" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="N18" s="6" t="n">
-        <v>3.537011899695518</v>
-      </c>
-      <c r="O18" s="7" t="inlineStr">
-        <is>
-          <t>AGCTCCATTGGTGGGTACACGCTCCG</t>
-        </is>
-      </c>
-      <c r="P18" s="6" t="n">
-        <v>64.22598535419934</v>
-      </c>
-      <c r="Q18" s="6" t="n">
-        <v>6.774014645800662</v>
-      </c>
-      <c r="R18" s="6" t="n">
-        <v>-0.7341697216033936</v>
-      </c>
-      <c r="S18" s="6" t="n">
-        <v>1.51e-06</v>
-      </c>
-      <c r="T18" s="6" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="U18" s="7" t="inlineStr">
-        <is>
-          <t>CTGGCTTAGTCTACGACATGGACGACATCTCCTATGTTCAGTTCTTGTGCGGCGAAGGCTACAACGCAACCACTCTAGCTCCATTGGTGGGTACACGCTCCGTGAGCTGTTCCTCCATTGTCCCTG</t>
-        </is>
-      </c>
-      <c r="V18" s="6" t="n">
-        <v>125</v>
-      </c>
-      <c r="W18" s="6" t="n">
-        <v>53.96825396825397</v>
-      </c>
-      <c r="X18" s="6" t="n">
-        <v>-6.521465301513672</v>
-      </c>
-      <c r="Y18" s="6" t="inlineStr"/>
-      <c r="Z18" s="6" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="inlineStr">
-        <is>
-          <t>CP002687.1</t>
-        </is>
-      </c>
-      <c r="B19" s="7" t="inlineStr">
-        <is>
-          <t>CCCAACAATCCAACTCACG</t>
-        </is>
-      </c>
-      <c r="C19" s="6" t="n">
-        <v>58.74250943646473</v>
-      </c>
-      <c r="D19" s="6" t="n">
-        <v>2.308298910148938</v>
-      </c>
-      <c r="E19" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="6" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="G19" s="6" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="H19" s="7" t="inlineStr">
-        <is>
-          <t>CCACCACTTTGAAGCTTCTC</t>
-        </is>
-      </c>
-      <c r="I19" s="6" t="n">
-        <v>58.87532172899461</v>
-      </c>
-      <c r="J19" s="6" t="n">
-        <v>2.625321728994606</v>
-      </c>
-      <c r="K19" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L19" s="6" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="M19" s="6" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="N19" s="6" t="n">
-        <v>4.933620639143545</v>
-      </c>
-      <c r="O19" s="7" t="inlineStr">
-        <is>
-          <t>CCGCCACCGTCCGAGCACCG</t>
-        </is>
-      </c>
-      <c r="P19" s="6" t="n">
-        <v>64.7335341111355</v>
-      </c>
-      <c r="Q19" s="6" t="n">
-        <v>0.2664658888645022</v>
-      </c>
-      <c r="R19" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S19" s="6" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="T19" s="6" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="U19" s="7" t="inlineStr">
-        <is>
-          <t>CCCAACAATCCAACTCACGTTGAGATCCGCCAAAACGTCCACATTGGCTGTGTTCAGGCGGAGAGTCACCAACGTGGGACCACCGTCGTCGGTCTACACCGCCACCGTCCGAGCACCGAAAGGAGTAGAAATCACGGTGGAGCCACAGAGTTTGTCATTTTCAAAGGCTTCACAAAAGAGAAGCTTCAAAGTGGTGGT</t>
-        </is>
-      </c>
-      <c r="V19" s="6" t="n">
-        <v>197</v>
-      </c>
-      <c r="W19" s="6" t="n">
-        <v>53.03030303030303</v>
-      </c>
-      <c r="X19" s="6" t="n">
-        <v>-17.26604652404785</v>
-      </c>
-      <c r="Y19" s="6" t="inlineStr"/>
-      <c r="Z19" s="6" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="inlineStr">
-        <is>
-          <t>CP002687.1</t>
-        </is>
-      </c>
-      <c r="B20" s="7" t="inlineStr">
-        <is>
-          <t>GAGCTGGAACATGTTCTGG</t>
-        </is>
-      </c>
-      <c r="C20" s="6" t="n">
-        <v>58.13313451624401</v>
-      </c>
-      <c r="D20" s="6" t="n">
-        <v>1.698923989928222</v>
-      </c>
-      <c r="E20" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="6" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="G20" s="6" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="H20" s="7" t="inlineStr">
-        <is>
-          <t>CACAGGGCTTGAGCAATTC</t>
-        </is>
-      </c>
-      <c r="I20" s="6" t="n">
-        <v>59.11187222956136</v>
-      </c>
-      <c r="J20" s="6" t="n">
-        <v>2.677661703245565</v>
-      </c>
-      <c r="K20" s="6" t="n">
-        <v>-0.790266752243042</v>
-      </c>
-      <c r="L20" s="6" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="M20" s="6" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="N20" s="6" t="n">
-        <v>4.376585693173787</v>
-      </c>
-      <c r="O20" s="7" t="inlineStr">
-        <is>
-          <t>ACGCGGCAAGGATCCTCCGGCT</t>
-        </is>
-      </c>
-      <c r="P20" s="6" t="n">
-        <v>64.70494890469467</v>
-      </c>
-      <c r="Q20" s="6" t="n">
-        <v>2.295051095305325</v>
-      </c>
-      <c r="R20" s="6" t="n">
-        <v>-0.9579751491546631</v>
-      </c>
-      <c r="S20" s="6" t="n">
-        <v>0.000168</v>
-      </c>
-      <c r="T20" s="6" t="inlineStr"/>
-      <c r="U20" s="7" t="inlineStr">
-        <is>
-          <t>GAGCTGGAACATGTTCTGGTTGCAGCCGGAGGATCCTTGCCGCGTTTACAATCTCTGTGGTCAATTAGGGTTTTGTAGCAGCGAATTGCTCAAGCCCTGTGC</t>
-        </is>
-      </c>
-      <c r="V20" s="6" t="n">
-        <v>101</v>
-      </c>
-      <c r="W20" s="6" t="n">
-        <v>51.9607843137255</v>
-      </c>
-      <c r="X20" s="6" t="n">
-        <v>-6.424409866333008</v>
-      </c>
-      <c r="Y20" s="6" t="inlineStr"/>
-      <c r="Z20" s="6" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="6" t="inlineStr">
-        <is>
-          <t>CP002687.1</t>
-        </is>
-      </c>
-      <c r="B21" s="7" t="inlineStr">
-        <is>
-          <t>GTATGCACGACTGGATCAC</t>
-        </is>
-      </c>
-      <c r="C21" s="6" t="n">
-        <v>58.01929187670885</v>
-      </c>
-      <c r="D21" s="6" t="n">
-        <v>1.585081350393057</v>
-      </c>
-      <c r="E21" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="6" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="G21" s="6" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="H21" s="7" t="inlineStr">
-        <is>
-          <t>GTAGTTGTCGAACCTGGTC</t>
-        </is>
-      </c>
-      <c r="I21" s="6" t="n">
-        <v>57.48615986233125</v>
-      </c>
-      <c r="J21" s="6" t="n">
-        <v>1.07962961135296</v>
-      </c>
-      <c r="K21" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L21" s="6" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="M21" s="6" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="N21" s="6" t="n">
-        <v>2.664710961746017</v>
-      </c>
-      <c r="O21" s="7" t="inlineStr">
-        <is>
-          <t>GCCGCCACACGCACGGAGGT</t>
-        </is>
-      </c>
-      <c r="P21" s="6" t="n">
-        <v>64.65986280657165</v>
-      </c>
-      <c r="Q21" s="6" t="n">
-        <v>0.3401371934283475</v>
-      </c>
-      <c r="R21" s="6" t="n">
-        <v>-1.617270469665527</v>
-      </c>
-      <c r="S21" s="6" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="T21" s="6" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="U21" s="7" t="inlineStr">
-        <is>
-          <t>GTATGCACGACTGGATCACTGAGAACCTCCGTGCGTGTGGCGGCACTTATCAGACATGTATCTGCGCCGTACCTTTCTTGGCAAAAAAGCAAGGTCTCGTGACCGTCACGTGCGATCCCAAGAACATCGAACACATGCTCAAGACCAGGTTCGACAACTACC</t>
-        </is>
-      </c>
-      <c r="V21" s="6" t="n">
-        <v>161</v>
-      </c>
-      <c r="W21" s="6" t="n">
-        <v>52.46913580246913</v>
-      </c>
-      <c r="X21" s="6" t="n">
-        <v>-10.59030723571777</v>
-      </c>
-      <c r="Y21" s="6" t="inlineStr"/>
-      <c r="Z21" s="6" t="inlineStr">
-        <is>
-          <t>43</t>
+          <t>161094</t>
         </is>
       </c>
     </row>

</xml_diff>